<commit_message>
Excel Cost Template worksheet
</commit_message>
<xml_diff>
--- a/Excel/DynamoDB+Cost+Template.xlsx
+++ b/Excel/DynamoDB+Cost+Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/amazon-dynamodb-tools/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE34E238-437E-DA44-B8D6-04585BEAAAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E4A32E-98BD-2847-A3E7-04FE80AF24CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="27320" windowHeight="16100" xr2:uid="{7EE89C3C-85C4-974C-9EC5-D0B4BF0B86AC}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>Time Unit List</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit size (KB) </t>
-  </si>
-  <si>
     <t xml:space="preserve">On Demand price per each unit consumed </t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   <si>
     <t xml:space="preserve"> Storage</t>
   </si>
+  <si>
+    <t>Unit size (KB) for reference</t>
+  </si>
 </sst>
 </file>
 
@@ -175,14 +175,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -256,6 +248,14 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -363,72 +363,74 @@
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +760,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,54 +775,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:7" s="11" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="2:7" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="18" t="s">
+    <row r="3" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="30">
+        <v>4</v>
+      </c>
+      <c r="D3" s="30">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <f>0.25/1000000</f>
         <v>2.4999999999999999E-7</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>1.25/1000000</f>
         <v>1.2500000000000001E-6</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8">
         <v>1.2999999999999999E-4</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>6.4999999999999997E-4</v>
       </c>
       <c r="E5" s="1"/>
@@ -829,149 +831,149 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="19">
+      <c r="B7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="18">
         <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <f>_xlfn.SWITCH(TimeUnit, "Year", 8760, "Month", 720, "Day", 24, "Hour", 1) * TimeUnitQty</f>
         <v>720</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="14">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <f>_xlfn.SWITCH(GT, "No", 1, "Yes, 2 regions", 2)</f>
         <v>1</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <f>_xlfn.SWITCH(GT, "No", 1, "Yes, 2 regions", 3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="E14" s="28" t="str">
+      <c r="B14" s="6"/>
+      <c r="E14" s="27" t="str">
         <f>"  Price per " &amp; TimeUnitQty &amp; " " &amp; TimeUnit &amp; " period:"</f>
         <v xml:space="preserve">  Price per 1 Month period:</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-    </row>
-    <row r="15" spans="2:7" s="7" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="20" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+    </row>
+    <row r="15" spans="2:7" s="6" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="G15" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="26" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="16" spans="2:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>100</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D16" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4">
         <f>C16*OnDemandRcuPrice*3600*Hours</f>
         <v>64.8</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <f>C16*ProvisionedPricePerReadUnitHourly*Hours*(1/(ProvisioningEfficiency/100))</f>
         <v>18.72</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="2:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>100</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="22">
+      <c r="D17" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="21">
         <f>C17*OnDemandWcuPrice*3600*Hours*GTWrites</f>
         <v>324</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="23">
         <f>C17*ProvisionedPricePerWriteUnitHourly*Hours*(1/(ProvisioningEfficiency/100))*GTWrites</f>
         <v>93.600000000000009</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="2:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="B18" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5">
         <v>100</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5">
+      <c r="D18" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4">
         <f>C18*StorageCostPerGbHour * (Hours/720)*GTStorage</f>
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="21" t="s">
-        <v>23</v>
+      <c r="B24" s="20" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:7" hidden="1" x14ac:dyDescent="0.2"/>
@@ -980,7 +982,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
@@ -988,7 +990,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
@@ -996,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:7" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update with new DynamoDB pricing
Updated the Calc to support the latest OnDemand DDB pricing
</commit_message>
<xml_diff>
--- a/Excel/DynamoDB+Cost+Template.xlsx
+++ b/Excel/DynamoDB+Cost+Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/amazon-dynamodb-tools/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irmit/Library/CloudStorage/WorkDocsDrive-Documents/Irmi/TFC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637BC981-68CE-E343-A4F1-CF6A946FAF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209DC081-EF65-2943-AF29-71D16A8A3420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19560" activeTab="2" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
   </bookViews>
   <sheets>
     <sheet name="CostSheet" sheetId="5" r:id="rId1"/>
@@ -138,7 +138,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Provisiond Capacity:</t>
         </r>
@@ -148,7 +147,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -159,49 +157,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Your Auto Scaling</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>target utilization (use 100% if AutoScaling</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> is disabled)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Your Auto Scaling target utilization (use 100% if AutoScaling is disabled)
 </t>
         </r>
         <r>
@@ -210,9 +167,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t xml:space="preserve">0%-100%.
+          <t xml:space="preserve">20%-90%.
 </t>
         </r>
         <r>
@@ -221,7 +177,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The default is 70%.
 </t>
@@ -232,7 +187,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">For example, if you choose 70% of your total capacity, it will add a buffer of 30% of your throughput to handle spikes. This implies that if you select 70 strongly consistent reads per second, the calculation will assume 100 strongly consistent reads per second (100 RCUs). 
 </t>
@@ -243,7 +197,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The higher the percentage you choose, the lower your cost will be. 
 </t>
@@ -254,7 +207,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -266,7 +218,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>On-Demand:</t>
         </r>
@@ -276,7 +227,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -287,7 +237,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The calculation determines the average percentage of the monthly capacity. For example, if you choose 50% and 100 strongly consistent reads per second, the calculation will assume you are requesting 50 requests per second for the entire month (50x3600cx730 = 131.4M requests per month).
 </t>
@@ -298,7 +247,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -309,7 +257,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">As a general rule, your utilization should be less than 18% of the provisioned capacity when using on-demand to save costs.
 </t>
@@ -320,7 +267,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -331,7 +277,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The higher the percentage you choose, the higher your cost will be. 
 </t>
@@ -342,7 +287,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t> </t>
         </r>
@@ -518,7 +462,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The sum of the percentage of eventual cosistancy, strong consistancy, and transaction reads </t>
         </r>
@@ -529,7 +472,6 @@
             <color rgb="FFFF0000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">must be equal to 100%. </t>
         </r>
@@ -539,7 +481,6 @@
             <color rgb="FFFF0000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -550,7 +491,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The default is 100% eventual consistency.</t>
         </r>
@@ -2195,21 +2135,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2325,6 +2250,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3695,56 +3633,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="173" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="173" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -3759,22 +3697,22 @@
     <xf numFmtId="2" fontId="12" fillId="5" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3786,6 +3724,96 @@
     <xf numFmtId="165" fontId="29" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3834,109 +3862,25 @@
     <xf numFmtId="164" fontId="14" fillId="6" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3951,10 +3895,10 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3969,16 +3913,10 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3988,6 +3926,306 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="62">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="0.00000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="0.00000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFBFBFBF"/>
@@ -4516,186 +4754,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="0.0000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="168" formatCode="0.0000000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4757,126 +4815,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="168" formatCode="0.0000000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0000000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0000000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0000000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0000000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.00000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.00000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6341,37 +6279,37 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D6EA7312-83FB-3648-A8CB-C88F5565BFA1}" name="Table4" displayName="Table4" ref="A2:S34" totalsRowCount="1">
   <autoFilter ref="A2:S33" xr:uid="{D6EA7312-83FB-3648-A8CB-C88F5565BFA1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N33">
-    <sortCondition descending="1" ref="A2:A33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S33">
+    <sortCondition ref="D2:D33"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{4F795EE2-B6FB-B742-8C31-9011902642B6}" name="# aws_region"/>
     <tableColumn id="2" xr3:uid="{CF4D784D-46E9-0C4C-81E2-62740353765A}" name="country_code"/>
     <tableColumn id="3" xr3:uid="{D47278EA-DC28-EA4F-9DFB-6558884EA6FA}" name="region_code"/>
     <tableColumn id="4" xr3:uid="{47C66DF7-3845-274F-9EA1-D5156FF306E8}" name="city"/>
-    <tableColumn id="6" xr3:uid="{4CA20C9C-C0C9-404C-A063-3757A6C99919}" name="Standard" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="15" xr3:uid="{3041EACD-1693-EC4F-9928-6C3936D206CE}" name="Standard_IA" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{EC65115E-728D-C840-BE66-3C6FD170968F}" name="Provisioned - WCU" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{E5D67E0F-AD04-A149-93D6-A3AF2ECE2F41}" name="Provisioned - RCU" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="10" xr3:uid="{63500D62-826A-BE41-A0E4-E4BC0A60313C}" name="Provisioned_IA- WCU" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{8B367489-BF7E-8B4F-9611-FA953AD6C79E}" name="Provisioned_IA- RCU" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{DF393429-B26C-0046-A59F-F50B43491C0C}" name="OD_WRU" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{772E548A-0178-ED47-9354-38D5057D5EBD}" name="OD_RRU" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{8B38EE2D-1D3C-9F4A-9EB7-08BD8A62CE3A}" name="OD_IA_WRU" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{FBA18991-3DBC-224E-B3CB-E81BC4ACEFC0}" name="OD_IA_RRU" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{E61725AA-8D5A-0242-B068-AFECA7F4B791}" name="Ratio_P_WCU" dataDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="6" xr3:uid="{4CA20C9C-C0C9-404C-A063-3757A6C99919}" name="Standard" dataDxfId="61" totalsRowDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{3041EACD-1693-EC4F-9928-6C3936D206CE}" name="Standard_IA" dataDxfId="60" totalsRowDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{EC65115E-728D-C840-BE66-3C6FD170968F}" name="Provisioned - WCU" dataDxfId="59" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E5D67E0F-AD04-A149-93D6-A3AF2ECE2F41}" name="Provisioned - RCU" dataDxfId="58" totalsRowDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{63500D62-826A-BE41-A0E4-E4BC0A60313C}" name="Provisioned_IA- WCU" dataDxfId="57" totalsRowDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{8B367489-BF7E-8B4F-9611-FA953AD6C79E}" name="Provisioned_IA- RCU" dataDxfId="56" totalsRowDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{DF393429-B26C-0046-A59F-F50B43491C0C}" name="OD_WRU" dataDxfId="55" totalsRowDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{772E548A-0178-ED47-9354-38D5057D5EBD}" name="OD_RRU" dataDxfId="54" totalsRowDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{8B38EE2D-1D3C-9F4A-9EB7-08BD8A62CE3A}" name="OD_IA_WRU" dataDxfId="53" totalsRowDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{FBA18991-3DBC-224E-B3CB-E81BC4ACEFC0}" name="OD_IA_RRU" dataDxfId="52" totalsRowDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{E61725AA-8D5A-0242-B068-AFECA7F4B791}" name="Ratio_P_WCU" dataDxfId="51" totalsRowDxfId="4">
       <calculatedColumnFormula>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{2B5D4F38-E0AF-9E43-8E63-3D8CCA639A89}" name="Ratio_P_RCU" dataDxfId="39" totalsRowDxfId="38">
+    <tableColumn id="18" xr3:uid="{2B5D4F38-E0AF-9E43-8E63-3D8CCA639A89}" name="Ratio_P_RCU" dataDxfId="50" totalsRowDxfId="3">
       <calculatedColumnFormula>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{44B28A4F-B169-BA49-A308-438B27B979B0}" name="RationOD_WCU" dataDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="19" xr3:uid="{44B28A4F-B169-BA49-A308-438B27B979B0}" name="RationOD_WCU" dataDxfId="49" totalsRowDxfId="2">
       <calculatedColumnFormula>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{401D964D-329D-F747-A4C3-8903B6AEB0CB}" name="RatioOD_RCU" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="20" xr3:uid="{401D964D-329D-F747-A4C3-8903B6AEB0CB}" name="RatioOD_RCU" dataDxfId="48" totalsRowDxfId="1">
       <calculatedColumnFormula>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{17D9228B-9461-7A44-879C-1782D7D904B9}" name="RatioStorage" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="21" xr3:uid="{17D9228B-9461-7A44-879C-1782D7D904B9}" name="RatioStorage" dataDxfId="47" totalsRowDxfId="0">
       <calculatedColumnFormula>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6678,14 +6616,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A5111F-7B7D-344C-A811-3E0902529217}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
@@ -6958,7 +6896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE6116E-4397-EA44-966F-6DDC633C7C56}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="G9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -6999,32 +6937,32 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="156"/>
-      <c r="G3" s="122" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
+      <c r="G3" s="152" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
     </row>
     <row r="4" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="157" t="s">
+      <c r="C4" s="134"/>
+      <c r="D4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="126"/>
       <c r="G4" s="41" t="s">
         <v>135</v>
       </c>
@@ -7039,15 +6977,15 @@
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="148">
+      <c r="B5" s="135">
         <v>1000</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="159" cm="1">
+      <c r="C5" s="136"/>
+      <c r="D5" s="127" cm="1">
         <f t="array" ref="D5">_xlfn.IFS(H4="Provisioned capacity",B5*I36,H4="On Demand",B5*M36)</f>
         <v>1251.0204081632655</v>
       </c>
-      <c r="E5" s="160"/>
+      <c r="E5" s="128"/>
       <c r="G5" s="41" t="s">
         <v>134</v>
       </c>
@@ -7063,40 +7001,40 @@
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="164">
+      <c r="B6" s="137">
         <v>100</v>
       </c>
-      <c r="C6" s="165"/>
-      <c r="D6" s="161">
+      <c r="C6" s="138"/>
+      <c r="D6" s="129">
         <f>B6*P36</f>
         <v>40</v>
       </c>
-      <c r="E6" s="143"/>
+      <c r="E6" s="130"/>
       <c r="G6" s="42" t="s">
         <v>131</v>
       </c>
       <c r="H6" s="56">
-        <v>2</v>
+        <v>1.44</v>
       </c>
       <c r="I6" s="59" t="str">
         <f>H6*1024&amp;(" Bytes")</f>
-        <v>2048 Bytes</v>
+        <v>1474.56 Bytes</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="166">
+      <c r="B7" s="139">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="167"/>
-      <c r="D7" s="162">
+      <c r="C7" s="140"/>
+      <c r="D7" s="131">
         <f>SUM(D5:D6)</f>
         <v>1291.0204081632655</v>
       </c>
-      <c r="E7" s="163"/>
+      <c r="E7" s="132"/>
       <c r="G7" s="37"/>
       <c r="H7" s="74" t="s">
         <v>122</v>
@@ -7223,7 +7161,7 @@
         <v>130</v>
       </c>
       <c r="H13" s="56">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="I13" s="59"/>
     </row>
@@ -7236,13 +7174,13 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="155"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="156"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
       <c r="G15" s="43" t="s">
         <v>124</v>
       </c>
@@ -7266,14 +7204,14 @@
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="147"/>
-      <c r="D16" s="138" t="s">
+      <c r="C16" s="134"/>
+      <c r="D16" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="139"/>
+      <c r="E16" s="142"/>
       <c r="G16" s="46" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.IFS($H$4="On Demand", "RRU", $H$4="Provisioned Capacity", "RCU")</f>
         <v>RCU</v>
@@ -7290,28 +7228,28 @@
         <f t="array" ref="J16">_xlfn.IFS($H$4="Provisioned Capacity",$I$16*$H$30,$H$4="On Demand",$I$16*$L$30/1000000)</f>
         <v>7.665</v>
       </c>
-      <c r="K16" s="136">
+      <c r="K16" s="166">
         <f>$J$16+$J$17</f>
         <v>160.965</v>
       </c>
-      <c r="L16" s="130">
+      <c r="L16" s="160">
         <f>$K$16+$K$18</f>
-        <v>160.965</v>
+        <v>182.19</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="148">
+      <c r="B17" s="135">
         <v>1251</v>
       </c>
-      <c r="C17" s="149"/>
-      <c r="D17" s="140" cm="1">
+      <c r="C17" s="136"/>
+      <c r="D17" s="143" cm="1">
         <f t="array" ref="D17">_xlfn.IFS(H4="Provisioned capacity",B17/I36,H4="On Demand",B17/M36)</f>
         <v>999.98368678629686</v>
       </c>
-      <c r="E17" s="141"/>
+      <c r="E17" s="144"/>
       <c r="G17" s="47" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.IFS($H$4="On Demand", "WRU", $H$4="Provisioned Capacity", "WCU")</f>
         <v>WCU</v>
@@ -7328,51 +7266,51 @@
         <f t="array" ref="J17">_xlfn.IFS($H$4="Provisioned Capacity",$I$17*$G$30,$H$4="On Demand",$I$17*$K$30/1000000)</f>
         <v>153.30000000000001</v>
       </c>
-      <c r="K17" s="137"/>
-      <c r="L17" s="131"/>
+      <c r="K17" s="167"/>
+      <c r="L17" s="161"/>
     </row>
     <row r="18" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="150">
+      <c r="B18" s="148">
         <v>200</v>
       </c>
-      <c r="C18" s="151"/>
-      <c r="D18" s="142">
+      <c r="C18" s="149"/>
+      <c r="D18" s="145">
         <f>B18/P36</f>
         <v>500</v>
       </c>
-      <c r="E18" s="143"/>
+      <c r="E18" s="130"/>
       <c r="G18" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="125">
+      <c r="H18" s="155">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="126"/>
-      <c r="J18" s="127"/>
+        <v>21.224999999999998</v>
+      </c>
+      <c r="I18" s="156"/>
+      <c r="J18" s="157"/>
       <c r="K18" s="45">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="132"/>
+        <v>21.224999999999998</v>
+      </c>
+      <c r="L18" s="162"/>
     </row>
     <row r="19" spans="1:16" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="152">
+      <c r="B19" s="150">
         <f>SUM(B17:B18)</f>
         <v>1451</v>
       </c>
-      <c r="C19" s="153"/>
-      <c r="D19" s="144">
+      <c r="C19" s="151"/>
+      <c r="D19" s="146">
         <f>SUM(D17:D18)</f>
         <v>1499.9836867862969</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="147"/>
       <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7449,13 +7387,13 @@
         <f t="array" ref="J21">_xlfn.IFS($H$4="Provisioned Capacity",$I$21*$J$30,$H$4="On Demand",$I$21*$N$30/1000000)</f>
         <v>9.5942857142857143</v>
       </c>
-      <c r="K21" s="136">
+      <c r="K21" s="166">
         <f>$J$21+$J$22</f>
         <v>201.27142857142857</v>
       </c>
-      <c r="L21" s="133">
+      <c r="L21" s="163">
         <f>$K$21+$K$23</f>
-        <v>201.27142857142857</v>
+        <v>209.76142857142858</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7481,24 +7419,24 @@
         <f t="array" ref="J22">_xlfn.IFS($H$4="Provisioned Capacity",$I$22*$I$30,$H$4="On Demand",$I$22*$M$30/1000000)</f>
         <v>191.67714285714285</v>
       </c>
-      <c r="K22" s="137"/>
-      <c r="L22" s="134"/>
+      <c r="K22" s="167"/>
+      <c r="L22" s="164"/>
     </row>
     <row r="23" spans="1:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="H23" s="128">
+      <c r="H23" s="158">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="126"/>
-      <c r="J23" s="127"/>
+        <v>8.49</v>
+      </c>
+      <c r="I23" s="156"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="45">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="135"/>
+        <v>8.49</v>
+      </c>
+      <c r="L23" s="165"/>
     </row>
     <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -7520,7 +7458,7 @@
       </c>
       <c r="H26" s="54" cm="1">
         <f t="array" ref="H26">_xlfn.IFS($G$26="Candidate to Standard",$L$21-$L$16,$G$26="Candidate to Standard-IA",$L$16-$L$21,$G$26="Even", 0)</f>
-        <v>40.306428571428569</v>
+        <v>27.571428571428584</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7582,19 +7520,19 @@
       </c>
       <c r="K30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],11,0)</f>
-        <v>1.4135</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="L30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],12,0)</f>
-        <v>0.28299999999999997</v>
+        <v>0.14149999999999999</v>
       </c>
       <c r="M30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],13,0)</f>
-        <v>1.7668999999999999</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="N30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],14,0)</f>
-        <v>0.35399999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O30" s="30">
         <f>VLOOKUP($H$5,Table4[#All],5,0)</f>
@@ -7618,7 +7556,7 @@
       </c>
       <c r="M35">
         <f>$M$30/$K$30</f>
-        <v>1.2500176865935619</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="N35">
         <f>$N$30/$L$30</f>
@@ -7629,19 +7567,19 @@
       <c r="H36" t="s">
         <v>132</v>
       </c>
-      <c r="I36" s="129">
+      <c r="I36" s="159">
         <f>$J$35*($H$11/($H$11+$H$12))+$I$35*($H$12/($H$12+$H$11))</f>
         <v>1.2510204081632654</v>
       </c>
-      <c r="J36" s="129"/>
+      <c r="J36" s="159"/>
       <c r="L36" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="129">
+      <c r="M36" s="159">
         <f>$N$35*($H$11/($H$11+$H$12))+$M$35*($H$12/($H$12+$H$11))</f>
-        <v>1.2504505394098553</v>
-      </c>
-      <c r="N36" s="129"/>
+        <v>1.2531012705811593</v>
+      </c>
+      <c r="N36" s="159"/>
       <c r="P36">
         <f>$P$30/$O$30</f>
         <v>0.4</v>
@@ -7652,6 +7590,23 @@
     <row r="40" spans="8:16" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -7662,91 +7617,74 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K16:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0.4166</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>41.66%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="13" operator="greaterThan">
       <formula>0.1333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="lessThanOrEqual">
       <formula>13.33%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="greaterThan">
       <formula>0.1333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="16" operator="lessThanOrEqual">
       <formula>13.33%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Candidate">
+    <cfRule type="containsText" dxfId="40" priority="9" operator="containsText" text="Candidate">
       <formula>NOT(ISERROR(SEARCH("Candidate",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="10" stopIfTrue="1" operator="containsText" text="Optimized">
+    <cfRule type="containsText" dxfId="39" priority="10" stopIfTrue="1" operator="containsText" text="Optimized">
       <formula>NOT(ISERROR(SEARCH("Optimized",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Optimized">
+    <cfRule type="containsText" dxfId="38" priority="7" operator="containsText" text="Optimized">
       <formula>NOT(ISERROR(SEARCH("Optimized",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Candidate">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="Candidate">
       <formula>NOT(ISERROR(SEARCH("Candidate",D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Candidate">
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="Candidate">
       <formula>NOT(ISERROR(SEARCH("Candidate",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" stopIfTrue="1" operator="containsText" text="Optimized">
+    <cfRule type="containsText" dxfId="31" priority="2" stopIfTrue="1" operator="containsText" text="Optimized">
       <formula>NOT(ISERROR(SEARCH("Optimized",G26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7778,7 +7716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF287C15-877C-2B4D-AD91-43E51C53AD46}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -7806,67 +7744,67 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="156"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
     </row>
     <row r="4" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="186"/>
-      <c r="D4" s="157" t="s">
+      <c r="C4" s="172"/>
+      <c r="D4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B5" s="183">
+      <c r="B5" s="168">
         <v>1000</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="185">
+      <c r="C5" s="169"/>
+      <c r="D5" s="170">
         <f>B5*1.25</f>
         <v>1250</v>
       </c>
-      <c r="E5" s="160"/>
+      <c r="E5" s="128"/>
     </row>
     <row r="6" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="177">
+      <c r="B6" s="179">
         <v>100</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179">
+      <c r="C6" s="180"/>
+      <c r="D6" s="181">
         <f>B6*0.4</f>
         <v>40</v>
       </c>
-      <c r="E6" s="180"/>
+      <c r="E6" s="182"/>
     </row>
     <row r="7" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="174">
+      <c r="B7" s="176">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="175"/>
-      <c r="D7" s="181">
+      <c r="C7" s="177"/>
+      <c r="D7" s="183">
         <f>SUM(D5:D6)</f>
         <v>1290</v>
       </c>
-      <c r="E7" s="182"/>
+      <c r="E7" s="184"/>
     </row>
     <row r="8" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -7949,67 +7887,67 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="155"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="156"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
     </row>
     <row r="16" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="168" t="s">
+      <c r="C16" s="141"/>
+      <c r="D16" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="139"/>
+      <c r="E16" s="142"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="169">
+      <c r="B17" s="185">
         <v>6000</v>
       </c>
-      <c r="C17" s="170"/>
-      <c r="D17" s="159">
+      <c r="C17" s="186"/>
+      <c r="D17" s="127">
         <f>B17/1.25</f>
         <v>4800</v>
       </c>
-      <c r="E17" s="160"/>
+      <c r="E17" s="128"/>
     </row>
     <row r="18" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="171">
+      <c r="B18" s="173">
         <v>168</v>
       </c>
-      <c r="C18" s="172"/>
-      <c r="D18" s="173">
+      <c r="C18" s="174"/>
+      <c r="D18" s="175">
         <f>B18/0.4</f>
         <v>420</v>
       </c>
-      <c r="E18" s="143"/>
+      <c r="E18" s="130"/>
     </row>
     <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="174">
+      <c r="B19" s="176">
         <f>SUM(B17:B18)</f>
         <v>6168</v>
       </c>
-      <c r="C19" s="175"/>
-      <c r="D19" s="176">
+      <c r="C19" s="177"/>
+      <c r="D19" s="178">
         <f>SUM(D17:D18)</f>
         <v>5220</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="147"/>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
@@ -8065,11 +8003,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B19:C19"/>
@@ -8083,58 +8016,63 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0.4166</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>41.66%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="greaterThan">
       <formula>0.1333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="lessThanOrEqual">
       <formula>13.33%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
       <formula>0.1333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThanOrEqual">
       <formula>13.33%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Candidate">
+    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="Candidate">
       <formula>NOT(ISERROR(SEARCH("Candidate",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" stopIfTrue="1" operator="containsText" text="Optimized">
+    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Optimized">
       <formula>NOT(ISERROR(SEARCH("Optimized",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Optimized">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Optimized">
       <formula>NOT(ISERROR(SEARCH("Optimized",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Candidate">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Candidate">
       <formula>NOT(ISERROR(SEARCH("Candidate",D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8147,8 +8085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE3DC98-ECA8-E340-8618-C286BC8288EE}">
   <dimension ref="A2:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8234,178 +8172,178 @@
     </row>
     <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="E3" s="27">
-        <v>0.25</v>
+        <v>0.33677000000000001</v>
       </c>
       <c r="F3" s="27">
-        <v>0.1</v>
+        <v>0.13471</v>
       </c>
       <c r="G3" s="26">
-        <v>6.4999999999999997E-4</v>
+        <v>8.7465000000000004E-4</v>
       </c>
       <c r="H3" s="26">
-        <v>1.2999999999999999E-4</v>
+        <v>1.7493000000000001E-4</v>
       </c>
       <c r="I3" s="26">
-        <v>8.0999999999999996E-4</v>
+        <v>9.6469999999999998E-4</v>
       </c>
       <c r="J3" s="26">
-        <v>1.6000000000000001E-4</v>
+        <v>2.187E-4</v>
       </c>
       <c r="K3" s="28">
-        <v>1.25</v>
+        <v>0.84</v>
       </c>
       <c r="L3" s="28">
-        <v>0.25</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="M3" s="28">
-        <v>1.56</v>
+        <v>1.05</v>
       </c>
       <c r="N3" s="28">
-        <v>0.31</v>
+        <v>0.21049999999999999</v>
       </c>
       <c r="O3" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2461538461538462</v>
+        <v>1.1029554679014462</v>
       </c>
       <c r="P3" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2307692307692311</v>
+        <v>1.2502143714628708</v>
       </c>
       <c r="Q3" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.248</v>
+        <v>1.25</v>
       </c>
       <c r="R3" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.24</v>
+        <v>1.2529761904761905</v>
       </c>
       <c r="S3" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.40000593877126822</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="E4" s="27">
-        <v>0.28000000000000003</v>
+        <v>0.3135</v>
       </c>
       <c r="F4" s="27">
-        <v>0.112</v>
+        <v>0.12540000000000001</v>
       </c>
       <c r="G4" s="26">
-        <v>7.2499999999999995E-4</v>
+        <v>8.1400000000000005E-4</v>
       </c>
       <c r="H4" s="26">
-        <v>1.45E-4</v>
+        <v>1.628E-4</v>
       </c>
       <c r="I4" s="26">
-        <v>9.0600000000000001E-4</v>
+        <v>1.018E-3</v>
       </c>
       <c r="J4" s="26">
-        <v>1.8100000000000001E-4</v>
+        <v>2.0350000000000001E-4</v>
       </c>
       <c r="K4" s="28">
-        <v>1.3942000000000001</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="L4" s="28">
-        <v>0.27900000000000003</v>
+        <v>0.155</v>
       </c>
       <c r="M4" s="28">
-        <v>1.7427999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="N4" s="28">
-        <v>0.34899999999999998</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="O4" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2496551724137932</v>
+        <v>1.2506142506142506</v>
       </c>
       <c r="P4" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2482758620689656</v>
+        <v>1.25</v>
       </c>
       <c r="Q4" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500358628604216</v>
+        <v>1.2484076433121019</v>
       </c>
       <c r="R4" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25089605734767</v>
+        <v>1.2580645161290323</v>
       </c>
       <c r="S4" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E5" s="27">
-        <v>0.3</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F5" s="27">
-        <v>0.12</v>
+        <v>0.114</v>
       </c>
       <c r="G5" s="26">
-        <v>7.7999999999999999E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H5" s="26">
-        <v>1.56E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I5" s="26">
-        <v>9.7499999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J5" s="26">
-        <v>1.95E-4</v>
+        <v>1.85E-4</v>
       </c>
       <c r="K5" s="28">
-        <v>1.5</v>
+        <v>0.71</v>
       </c>
       <c r="L5" s="28">
-        <v>0.3</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M5" s="28">
-        <v>1.875</v>
+        <v>0.89</v>
       </c>
       <c r="N5" s="28">
-        <v>0.375</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O5" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P5" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
@@ -8413,11 +8351,11 @@
       </c>
       <c r="Q5" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R5" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S5" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8426,62 +8364,62 @@
     </row>
     <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E6" s="27">
-        <v>0.3</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F6" s="27">
-        <v>0.12</v>
+        <v>0.114</v>
       </c>
       <c r="G6" s="26">
-        <v>7.7999999999999999E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H6" s="26">
-        <v>1.56E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I6" s="26">
-        <v>9.7499999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J6" s="26">
-        <v>1.95E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K6" s="28">
-        <v>1.5</v>
+        <v>0.71</v>
       </c>
       <c r="L6" s="28">
-        <v>0.3</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M6" s="28">
-        <v>1.875</v>
+        <v>0.89</v>
       </c>
       <c r="N6" s="28">
-        <v>0.375</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O6" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P6" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q6" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R6" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S6" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8490,62 +8428,62 @@
     </row>
     <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="E7" s="27">
-        <v>0.25</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F7" s="27">
-        <v>0.1</v>
+        <v>0.114</v>
       </c>
       <c r="G7" s="26">
-        <v>6.4999999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H7" s="26">
-        <v>1.2999999999999999E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I7" s="26">
-        <v>8.0999999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J7" s="26">
-        <v>1.6000000000000001E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K7" s="28">
-        <v>1.25</v>
+        <v>0.71</v>
       </c>
       <c r="L7" s="28">
-        <v>0.25</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M7" s="28">
-        <v>1.56</v>
+        <v>0.89</v>
       </c>
       <c r="N7" s="28">
-        <v>0.31</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O7" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2461538461538462</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P7" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2307692307692311</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q7" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.248</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R7" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.24</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S7" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8554,62 +8492,62 @@
     </row>
     <row r="8" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E8" s="27">
-        <v>0.25</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F8" s="27">
-        <v>0.1</v>
+        <v>0.114</v>
       </c>
       <c r="G8" s="26">
-        <v>6.4999999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H8" s="26">
-        <v>1.2999999999999999E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I8" s="26">
-        <v>8.0999999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J8" s="26">
-        <v>1.6000000000000001E-4</v>
+        <v>1.85E-4</v>
       </c>
       <c r="K8" s="28">
-        <v>1.25</v>
+        <v>0.71</v>
       </c>
       <c r="L8" s="28">
-        <v>0.25</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M8" s="28">
-        <v>1.56</v>
+        <v>0.89</v>
       </c>
       <c r="N8" s="28">
-        <v>0.31</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O8" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2461538461538462</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P8" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2307692307692311</v>
+        <v>1.25</v>
       </c>
       <c r="Q8" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.248</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R8" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.24</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S8" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8618,302 +8556,302 @@
     </row>
     <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="E9" s="27">
-        <v>0.375</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F9" s="27">
-        <v>0.15</v>
+        <v>0.114</v>
       </c>
       <c r="G9" s="26">
-        <v>9.7499999999999996E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="H9" s="26">
-        <v>1.95E-4</v>
+        <v>1.484E-4</v>
       </c>
       <c r="I9" s="26">
-        <v>1.219E-3</v>
+        <v>9.2800000000000001E-4</v>
       </c>
       <c r="J9" s="26">
-        <v>2.4399999999999999E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K9" s="28">
-        <v>1.875</v>
+        <v>0.71</v>
       </c>
       <c r="L9" s="28">
-        <v>0.375</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M9" s="28">
-        <v>2.3439999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="N9" s="28">
-        <v>0.46899999999999997</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O9" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2502564102564104</v>
+        <v>1.2506738544474394</v>
       </c>
       <c r="P9" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2512820512820513</v>
+        <v>1.25</v>
       </c>
       <c r="Q9" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2501333333333333</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R9" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2506666666666666</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S9" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E10" s="27">
-        <v>0.31130000000000002</v>
+        <v>0.27074999999999999</v>
       </c>
       <c r="F10" s="27">
-        <v>0.1245</v>
+        <v>0.10829999999999999</v>
       </c>
       <c r="G10" s="26">
-        <v>8.0849999999999997E-4</v>
+        <v>7.0489999999999995E-4</v>
       </c>
       <c r="H10" s="26">
-        <v>1.617E-4</v>
+        <v>1.4098E-4</v>
       </c>
       <c r="I10" s="26">
-        <v>1.0106E-3</v>
+        <v>8.811E-4</v>
       </c>
       <c r="J10" s="26">
-        <v>2.0210000000000001E-4</v>
+        <v>1.762E-4</v>
       </c>
       <c r="K10" s="28">
-        <v>1.5548999999999999</v>
-      </c>
-      <c r="L10" s="28">
-        <v>0.311</v>
+        <v>0.68</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0.13550000000000001</v>
       </c>
       <c r="M10" s="28">
-        <v>1.9436</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="N10" s="28">
-        <v>0.38900000000000001</v>
+        <v>0.16950000000000001</v>
       </c>
       <c r="O10" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2499690785405071</v>
+        <v>1.2499645339764507</v>
       </c>
       <c r="P10" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2498453927025357</v>
+        <v>1.2498226698822528</v>
       </c>
       <c r="Q10" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499839217956139</v>
+        <v>1.2426470588235292</v>
       </c>
       <c r="R10" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508038585209003</v>
+        <v>1.2509225092250922</v>
       </c>
       <c r="S10" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39993575329264375</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="E11" s="27">
-        <v>0.31130000000000002</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F11" s="27">
-        <v>0.12452000000000001</v>
+        <v>0.114</v>
       </c>
       <c r="G11" s="26">
-        <v>8.0849999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H11" s="26">
-        <v>1.617E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I11" s="26">
-        <v>1.0108999999999999E-3</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J11" s="26">
-        <v>2.0239999999999999E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K11" s="28">
-        <v>1.5509999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="L11" s="28">
-        <v>0.31130000000000002</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M11" s="28">
-        <v>1.9470000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="N11" s="28">
-        <v>0.38940000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O11" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P11" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721087</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q11" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2553191489361704</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R11" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508833922261484</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S11" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E12" s="27">
-        <v>0.33960000000000001</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F12" s="27">
-        <v>0.13583999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="G12" s="26">
-        <v>8.8199999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H12" s="26">
-        <v>1.7640000000000001E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I12" s="26">
-        <v>1.1027999999999999E-3</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J12" s="26">
-        <v>2.208E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K12" s="28">
-        <v>1.6961999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="L12" s="28">
-        <v>0.33960000000000001</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M12" s="28">
-        <v>2.1202999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="N12" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O12" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P12" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721089</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q12" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500294776559369</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R12" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.0424028268551235</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S12" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E13" s="27">
-        <v>0.29715000000000003</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F13" s="27">
-        <v>0.11885999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="G13" s="26">
-        <v>7.7200000000000001E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="H13" s="26">
-        <v>1.5440000000000001E-4</v>
+        <v>1.484E-4</v>
       </c>
       <c r="I13" s="26">
-        <v>9.6500000000000004E-4</v>
+        <v>9.2750000000000005E-4</v>
       </c>
       <c r="J13" s="26">
-        <v>1.93E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K13" s="28">
-        <v>1.4845999999999999</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="L13" s="28">
-        <v>0.29699999999999999</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M13" s="28">
-        <v>1.8557999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="N13" s="28">
-        <v>0.371</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O13" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
@@ -8925,59 +8863,59 @@
       </c>
       <c r="Q13" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500336791054829</v>
+        <v>1.2447552447552448</v>
       </c>
       <c r="R13" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2491582491582491</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S13" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E14" s="27">
-        <v>0.29715000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="F14" s="27">
-        <v>0.11885999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="G14" s="26">
-        <v>7.7200000000000001E-4</v>
+        <v>7.7999999999999999E-4</v>
       </c>
       <c r="H14" s="26">
-        <v>1.5440000000000001E-4</v>
+        <v>1.56E-4</v>
       </c>
       <c r="I14" s="26">
-        <v>9.6500000000000004E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="J14" s="26">
-        <v>1.93E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="K14" s="28">
-        <v>1.4845999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="L14" s="28">
-        <v>0.29699999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="M14" s="28">
-        <v>1.8557999999999999</v>
+        <v>0.9375</v>
       </c>
       <c r="N14" s="28">
-        <v>0.371</v>
+        <v>0.1875</v>
       </c>
       <c r="O14" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
@@ -8989,75 +8927,75 @@
       </c>
       <c r="Q14" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500336791054829</v>
+        <v>1.25</v>
       </c>
       <c r="R14" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2491582491582491</v>
+        <v>1.25</v>
       </c>
       <c r="S14" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E15" s="27">
-        <v>0.28299999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="F15" s="27">
-        <v>0.1132</v>
+        <v>0.12</v>
       </c>
       <c r="G15" s="26">
-        <v>7.3499999999999998E-4</v>
+        <v>7.7999999999999999E-4</v>
       </c>
       <c r="H15" s="26">
-        <v>1.47E-4</v>
+        <v>1.56E-4</v>
       </c>
       <c r="I15" s="26">
-        <v>9.19E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="J15" s="26">
-        <v>1.84E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="K15" s="28">
-        <v>1.4135</v>
+        <v>0.75</v>
       </c>
       <c r="L15" s="28">
-        <v>0.28299999999999997</v>
+        <v>0.15</v>
       </c>
       <c r="M15" s="28">
-        <v>1.7668999999999999</v>
+        <v>0.9375</v>
       </c>
       <c r="N15" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.1875</v>
       </c>
       <c r="O15" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.25</v>
       </c>
       <c r="P15" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721089</v>
+        <v>1.25</v>
       </c>
       <c r="Q15" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500176865935619</v>
+        <v>1.25</v>
       </c>
       <c r="R15" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508833922261484</v>
+        <v>1.25</v>
       </c>
       <c r="S15" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9066,126 +9004,126 @@
     </row>
     <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E16" s="27">
-        <v>0.28299999999999997</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F16" s="27">
-        <v>0.1132</v>
+        <v>0.11</v>
       </c>
       <c r="G16" s="26">
-        <v>7.3499999999999998E-4</v>
+        <v>7.1500000000000003E-4</v>
       </c>
       <c r="H16" s="26">
-        <v>1.47E-4</v>
+        <v>1.4300000000000001E-4</v>
       </c>
       <c r="I16" s="26">
-        <v>9.19E-4</v>
+        <v>8.9400000000000005E-4</v>
       </c>
       <c r="J16" s="26">
-        <v>1.84E-4</v>
+        <v>1.7899999999999999E-4</v>
       </c>
       <c r="K16" s="28">
-        <v>1.4135</v>
+        <v>0.6875</v>
       </c>
       <c r="L16" s="28">
-        <v>0.28299999999999997</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M16" s="28">
-        <v>1.7668999999999999</v>
+        <v>0.85950000000000004</v>
       </c>
       <c r="N16" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="O16" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.2503496503496503</v>
       </c>
       <c r="P16" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721089</v>
+        <v>1.2517482517482517</v>
       </c>
       <c r="Q16" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500176865935619</v>
+        <v>1.2501818181818183</v>
       </c>
       <c r="R16" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508833922261484</v>
+        <v>1.2509090909090907</v>
       </c>
       <c r="S16" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="E17" s="27">
-        <v>0.29715000000000003</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F17" s="27">
-        <v>0.11885999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="G17" s="26">
-        <v>7.7174999999999998E-4</v>
+        <v>7.1500000000000003E-4</v>
       </c>
       <c r="H17" s="26">
-        <v>1.5435000000000001E-4</v>
+        <v>1.4300000000000001E-4</v>
       </c>
       <c r="I17" s="26">
-        <v>9.6469999999999998E-4</v>
+        <v>8.9400000000000005E-4</v>
       </c>
       <c r="J17" s="26">
-        <v>1.93E-4</v>
+        <v>1.7899999999999999E-4</v>
       </c>
       <c r="K17" s="28">
-        <v>1.4842</v>
+        <v>0.6875</v>
       </c>
       <c r="L17" s="28">
-        <v>0.29680000000000001</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M17" s="28">
-        <v>1.8552999999999999</v>
+        <v>0.85950000000000004</v>
       </c>
       <c r="N17" s="28">
-        <v>0.371</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="O17" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2500161969549726</v>
+        <v>1.2503496503496503</v>
       </c>
       <c r="P17" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2504049238743116</v>
+        <v>1.2517482517482517</v>
       </c>
       <c r="Q17" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500336881821856</v>
+        <v>1.2501818181818183</v>
       </c>
       <c r="R17" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25</v>
+        <v>1.2509090909090907</v>
       </c>
       <c r="S17" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9194,62 +9132,62 @@
     </row>
     <row r="18" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E18" s="27">
-        <v>0.26900000000000002</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="F18" s="27">
-        <v>0.1076</v>
+        <v>0.12239999999999999</v>
       </c>
       <c r="G18" s="26">
-        <v>6.9800000000000005E-4</v>
+        <v>7.9299999999999998E-4</v>
       </c>
       <c r="H18" s="26">
-        <v>1.3999999999999999E-4</v>
+        <v>1.5860000000000001E-4</v>
       </c>
       <c r="I18" s="26">
-        <v>8.7250000000000001E-4</v>
+        <v>9.9099999999999991E-4</v>
       </c>
       <c r="J18" s="26">
-        <v>1.75E-4</v>
+        <v>1.983E-4</v>
       </c>
       <c r="K18" s="28">
-        <v>1.3428</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="L18" s="28">
-        <v>0.26900000000000002</v>
+        <v>0.1525</v>
       </c>
       <c r="M18" s="28">
-        <v>1.6785000000000001</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="N18" s="28">
-        <v>0.33600000000000002</v>
+        <v>0.1905</v>
       </c>
       <c r="O18" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2496847414880201</v>
       </c>
       <c r="P18" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2503152585119797</v>
       </c>
       <c r="Q18" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.2524590163934426</v>
       </c>
       <c r="R18" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2490706319702602</v>
+        <v>1.2491803278688525</v>
       </c>
       <c r="S18" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9258,62 +9196,62 @@
     </row>
     <row r="19" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="E19" s="27">
-        <v>0.33660000000000001</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="F19" s="27">
-        <v>0.13464000000000001</v>
+        <v>0.1132</v>
       </c>
       <c r="G19" s="26">
-        <v>8.7200000000000005E-4</v>
+        <v>7.3499999999999998E-4</v>
       </c>
       <c r="H19" s="26">
-        <v>1.75E-4</v>
+        <v>1.47E-4</v>
       </c>
       <c r="I19" s="26">
-        <v>1.0901000000000001E-3</v>
+        <v>9.19E-4</v>
       </c>
       <c r="J19" s="26">
-        <v>2.1800000000000001E-4</v>
+        <v>1.84E-4</v>
       </c>
       <c r="K19" s="28">
-        <v>1.67</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="L19" s="28">
-        <v>0.33600000000000002</v>
+        <v>0.14149999999999999</v>
       </c>
       <c r="M19" s="28">
-        <v>2.101</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="N19" s="28">
-        <v>0.41899999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O19" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2501146788990827</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P19" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2457142857142858</v>
+        <v>1.2517006802721089</v>
       </c>
       <c r="Q19" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2580838323353294</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="R19" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2470238095238093</v>
+        <v>1.2508833922261484</v>
       </c>
       <c r="S19" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9322,62 +9260,62 @@
     </row>
     <row r="20" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E20" s="27">
-        <v>0.30599999999999999</v>
+        <v>0.29715000000000003</v>
       </c>
       <c r="F20" s="27">
-        <v>0.12239999999999999</v>
+        <v>0.11885999999999999</v>
       </c>
       <c r="G20" s="26">
-        <v>7.9299999999999998E-4</v>
+        <v>7.7200000000000001E-4</v>
       </c>
       <c r="H20" s="26">
-        <v>1.5860000000000001E-4</v>
+        <v>1.5440000000000001E-4</v>
       </c>
       <c r="I20" s="26">
-        <v>9.9099999999999991E-4</v>
+        <v>9.6500000000000004E-4</v>
       </c>
       <c r="J20" s="26">
-        <v>1.983E-4</v>
+        <v>1.93E-4</v>
       </c>
       <c r="K20" s="28">
-        <v>1.5249999999999999</v>
+        <v>0.74229999999999996</v>
       </c>
       <c r="L20" s="28">
-        <v>0.30499999999999999</v>
+        <v>0.1487</v>
       </c>
       <c r="M20" s="28">
-        <v>1.91</v>
+        <v>0.92789999999999995</v>
       </c>
       <c r="N20" s="28">
-        <v>0.38100000000000001</v>
+        <v>0.18559999999999999</v>
       </c>
       <c r="O20" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2496847414880201</v>
+        <v>1.25</v>
       </c>
       <c r="P20" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2503152585119797</v>
+        <v>1.25</v>
       </c>
       <c r="Q20" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2524590163934426</v>
+        <v>1.2500336791054829</v>
       </c>
       <c r="R20" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2491803278688525</v>
+        <v>1.2481506388702084</v>
       </c>
       <c r="S20" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9386,62 +9324,62 @@
     </row>
     <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E21" s="27">
-        <v>0.27500000000000002</v>
+        <v>0.29715000000000003</v>
       </c>
       <c r="F21" s="27">
-        <v>0.11</v>
+        <v>0.11885999999999999</v>
       </c>
       <c r="G21" s="26">
-        <v>7.1500000000000003E-4</v>
+        <v>7.7174999999999998E-4</v>
       </c>
       <c r="H21" s="26">
-        <v>1.4300000000000001E-4</v>
+        <v>1.5435000000000001E-4</v>
       </c>
       <c r="I21" s="26">
-        <v>8.9400000000000005E-4</v>
+        <v>9.6469999999999998E-4</v>
       </c>
       <c r="J21" s="26">
-        <v>1.7899999999999999E-4</v>
+        <v>1.93E-4</v>
       </c>
       <c r="K21" s="28">
-        <v>1.375</v>
+        <v>0.74</v>
       </c>
       <c r="L21" s="28">
-        <v>0.27500000000000002</v>
+        <v>0.1484</v>
       </c>
       <c r="M21" s="28">
-        <v>1.7190000000000001</v>
+        <v>0.92764999999999997</v>
       </c>
       <c r="N21" s="28">
-        <v>0.34399999999999997</v>
+        <v>0.1855</v>
       </c>
       <c r="O21" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503496503496503</v>
+        <v>1.2500161969549726</v>
       </c>
       <c r="P21" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517482517482517</v>
+        <v>1.2504049238743116</v>
       </c>
       <c r="Q21" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2501818181818183</v>
+        <v>1.253581081081081</v>
       </c>
       <c r="R21" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2509090909090907</v>
+        <v>1.25</v>
       </c>
       <c r="S21" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9450,62 +9388,62 @@
     </row>
     <row r="22" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E22" s="27">
-        <v>0.27500000000000002</v>
+        <v>0.29715000000000003</v>
       </c>
       <c r="F22" s="27">
-        <v>0.11</v>
+        <v>0.11885999999999999</v>
       </c>
       <c r="G22" s="26">
-        <v>7.1500000000000003E-4</v>
+        <v>7.7200000000000001E-4</v>
       </c>
       <c r="H22" s="26">
-        <v>1.4300000000000001E-4</v>
+        <v>1.5440000000000001E-4</v>
       </c>
       <c r="I22" s="26">
-        <v>8.9400000000000005E-4</v>
+        <v>9.6500000000000004E-4</v>
       </c>
       <c r="J22" s="26">
-        <v>1.7899999999999999E-4</v>
+        <v>1.93E-4</v>
       </c>
       <c r="K22" s="28">
-        <v>1.375</v>
+        <v>0.74229999999999996</v>
       </c>
       <c r="L22" s="28">
-        <v>0.27500000000000002</v>
+        <v>0.1487</v>
       </c>
       <c r="M22" s="28">
-        <v>1.7190000000000001</v>
+        <v>0.92789999999999995</v>
       </c>
       <c r="N22" s="28">
-        <v>0.34399999999999997</v>
+        <v>0.18559999999999999</v>
       </c>
       <c r="O22" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503496503496503</v>
+        <v>1.25</v>
       </c>
       <c r="P22" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517482517482517</v>
+        <v>1.25</v>
       </c>
       <c r="Q22" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2501818181818183</v>
+        <v>1.2500336791054829</v>
       </c>
       <c r="R22" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2509090909090907</v>
+        <v>1.2481506388702084</v>
       </c>
       <c r="S22" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9514,62 +9452,62 @@
     </row>
     <row r="23" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="F23" s="27">
-        <v>0.114</v>
+        <v>0.1132</v>
       </c>
       <c r="G23" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>7.3499999999999998E-4</v>
       </c>
       <c r="H23" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.47E-4</v>
       </c>
       <c r="I23" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>9.19E-4</v>
       </c>
       <c r="J23" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>1.84E-4</v>
       </c>
       <c r="K23" s="28">
-        <v>1.4231</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="L23" s="28">
-        <v>0.28460000000000002</v>
+        <v>0.14149999999999999</v>
       </c>
       <c r="M23" s="28">
-        <v>1.7788999999999999</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="N23" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O23" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P23" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.2517006802721089</v>
       </c>
       <c r="Q23" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="R23" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508784258608572</v>
+        <v>1.2508833922261484</v>
       </c>
       <c r="S23" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9578,126 +9516,126 @@
     </row>
     <row r="24" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E24" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="F24" s="27">
-        <v>0.114</v>
+        <v>0.1076</v>
       </c>
       <c r="G24" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>6.9800000000000005E-4</v>
       </c>
       <c r="H24" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="I24" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>8.7250000000000001E-4</v>
       </c>
       <c r="J24" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>1.75E-4</v>
       </c>
       <c r="K24" s="28">
-        <v>1.4231</v>
+        <v>0.67</v>
       </c>
       <c r="L24" s="28">
-        <v>0.28460000000000002</v>
+        <v>0.13450000000000001</v>
       </c>
       <c r="M24" s="28">
-        <v>1.7788999999999999</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="N24" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="O24" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.25</v>
       </c>
       <c r="P24" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.25</v>
       </c>
       <c r="Q24" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2447761194029849</v>
       </c>
       <c r="R24" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508784258608572</v>
+        <v>1.2490706319702602</v>
       </c>
       <c r="S24" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="E25" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.33660000000000001</v>
       </c>
       <c r="F25" s="27">
-        <v>0.114</v>
+        <v>0.13464000000000001</v>
       </c>
       <c r="G25" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.7200000000000005E-4</v>
       </c>
       <c r="H25" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.75E-4</v>
       </c>
       <c r="I25" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.0901000000000001E-3</v>
       </c>
       <c r="J25" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>2.1800000000000001E-4</v>
       </c>
       <c r="K25" s="28">
-        <v>1.4231</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="L25" s="28">
-        <v>0.28460000000000002</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="M25" s="28">
-        <v>1.7788999999999999</v>
+        <v>1.0505</v>
       </c>
       <c r="N25" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.20949999999999999</v>
       </c>
       <c r="O25" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2501146788990827</v>
       </c>
       <c r="P25" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.2457142857142858</v>
       </c>
       <c r="Q25" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2580838323353294</v>
       </c>
       <c r="R25" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508784258608572</v>
+        <v>1.2470238095238093</v>
       </c>
       <c r="S25" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9706,382 +9644,382 @@
     </row>
     <row r="26" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="E26" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.33960000000000001</v>
       </c>
       <c r="F26" s="27">
-        <v>0.114</v>
+        <v>0.13583999999999999</v>
       </c>
       <c r="G26" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.8199999999999997E-4</v>
       </c>
       <c r="H26" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.7640000000000001E-4</v>
       </c>
       <c r="I26" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.1027999999999999E-3</v>
       </c>
       <c r="J26" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>2.208E-4</v>
       </c>
       <c r="K26" s="28">
-        <v>1.4231</v>
+        <v>0.85</v>
       </c>
       <c r="L26" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.17</v>
       </c>
       <c r="M26" s="28">
-        <v>1.7788999999999999</v>
+        <v>1.06</v>
       </c>
       <c r="N26" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O26" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P26" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.2517006802721089</v>
       </c>
       <c r="Q26" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2470588235294118</v>
       </c>
       <c r="R26" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.0411764705882351</v>
       </c>
       <c r="S26" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E27" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.31130000000000002</v>
       </c>
       <c r="F27" s="27">
-        <v>0.114</v>
+        <v>0.1245</v>
       </c>
       <c r="G27" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.0849999999999997E-4</v>
       </c>
       <c r="H27" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.617E-4</v>
       </c>
       <c r="I27" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.0106E-3</v>
       </c>
       <c r="J27" s="26">
-        <v>1.85E-4</v>
+        <v>2.0210000000000001E-4</v>
       </c>
       <c r="K27" s="28">
-        <v>1.42</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="L27" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.1555</v>
       </c>
       <c r="M27" s="28">
-        <v>1.78</v>
+        <v>0.97</v>
       </c>
       <c r="N27" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.19450000000000001</v>
       </c>
       <c r="O27" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2499690785405071</v>
       </c>
       <c r="P27" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2498453927025357</v>
       </c>
       <c r="Q27" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2535211267605635</v>
+        <v>1.2516129032258063</v>
       </c>
       <c r="R27" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.2508038585209003</v>
       </c>
       <c r="S27" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39993575329264375</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="E28" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.31130000000000002</v>
       </c>
       <c r="F28" s="27">
-        <v>0.114</v>
+        <v>0.12452000000000001</v>
       </c>
       <c r="G28" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.0849999999999997E-4</v>
       </c>
       <c r="H28" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.617E-4</v>
       </c>
       <c r="I28" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.0108999999999999E-3</v>
       </c>
       <c r="J28" s="26">
-        <v>1.85E-4</v>
+        <v>2.0239999999999999E-4</v>
       </c>
       <c r="K28" s="28">
-        <v>1.4231</v>
+        <v>0.77549999999999997</v>
       </c>
       <c r="L28" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.15565000000000001</v>
       </c>
       <c r="M28" s="28">
-        <v>1.7788999999999999</v>
+        <v>0.97350000000000003</v>
       </c>
       <c r="N28" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.19450000000000001</v>
       </c>
       <c r="O28" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P28" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2517006802721087</v>
       </c>
       <c r="Q28" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="R28" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.2495984580790234</v>
       </c>
       <c r="S28" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E29" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.375</v>
       </c>
       <c r="F29" s="27">
-        <v>0.114</v>
+        <v>0.15</v>
       </c>
       <c r="G29" s="26">
-        <v>7.4200000000000004E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="H29" s="26">
-        <v>1.484E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="I29" s="26">
-        <v>9.2800000000000001E-4</v>
+        <v>1.219E-3</v>
       </c>
       <c r="J29" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>2.4399999999999999E-4</v>
       </c>
       <c r="K29" s="28">
-        <v>1.4269000000000001</v>
+        <v>0.9375</v>
       </c>
       <c r="L29" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.1875</v>
       </c>
       <c r="M29" s="28">
-        <v>1.7836000000000001</v>
+        <v>1.1719999999999999</v>
       </c>
       <c r="N29" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.23449999999999999</v>
       </c>
       <c r="O29" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2506738544474394</v>
+        <v>1.2502564102564104</v>
       </c>
       <c r="P29" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2512820512820513</v>
       </c>
       <c r="Q29" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499824795010162</v>
+        <v>1.2501333333333333</v>
       </c>
       <c r="R29" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.2506666666666666</v>
       </c>
       <c r="S29" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E30" s="27">
-        <v>0.27074999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="F30" s="27">
-        <v>0.10829999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="G30" s="26">
-        <v>7.0489999999999995E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H30" s="26">
-        <v>1.4098E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I30" s="26">
-        <v>8.811E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J30" s="26">
-        <v>1.762E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K30" s="28">
-        <v>1.3555999999999999</v>
-      </c>
-      <c r="L30" s="29">
-        <v>0.27100000000000002</v>
+        <v>0.625</v>
+      </c>
+      <c r="L30" s="28">
+        <v>0.125</v>
       </c>
       <c r="M30" s="28">
-        <v>1.6944999999999999</v>
+        <v>0.78</v>
       </c>
       <c r="N30" s="28">
-        <v>0.33900000000000002</v>
+        <v>0.155</v>
       </c>
       <c r="O30" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2499645339764507</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="P30" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2498226698822528</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="Q30" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.248</v>
       </c>
       <c r="R30" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2509225092250922</v>
+        <v>1.24</v>
       </c>
       <c r="S30" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E31" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="F31" s="27">
-        <v>0.114</v>
+        <v>0.1</v>
       </c>
       <c r="G31" s="26">
-        <v>7.4200000000000004E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H31" s="26">
-        <v>1.484E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I31" s="26">
-        <v>9.2750000000000005E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J31" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K31" s="28">
-        <v>1.4269000000000001</v>
+        <v>0.625</v>
       </c>
       <c r="L31" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="M31" s="28">
-        <v>1.7836000000000001</v>
+        <v>0.78</v>
       </c>
       <c r="N31" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="O31" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="P31" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="Q31" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499824795010162</v>
+        <v>1.248</v>
       </c>
       <c r="R31" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.24</v>
       </c>
       <c r="S31" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -10090,130 +10028,130 @@
     </row>
     <row r="32" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E32" s="27">
-        <v>0.3135</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F32" s="27">
-        <v>0.12540000000000001</v>
+        <v>0.112</v>
       </c>
       <c r="G32" s="26">
-        <v>8.1400000000000005E-4</v>
+        <v>7.2499999999999995E-4</v>
       </c>
       <c r="H32" s="26">
-        <v>1.628E-4</v>
+        <v>1.45E-4</v>
       </c>
       <c r="I32" s="26">
-        <v>1.018E-3</v>
+        <v>9.0600000000000001E-4</v>
       </c>
       <c r="J32" s="26">
-        <v>2.0350000000000001E-4</v>
+        <v>1.8100000000000001E-4</v>
       </c>
       <c r="K32" s="28">
-        <v>1.57</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="L32" s="28">
-        <v>0.31</v>
+        <v>0.13950000000000001</v>
       </c>
       <c r="M32" s="28">
-        <v>1.96</v>
+        <v>0.87</v>
       </c>
       <c r="N32" s="28">
-        <v>0.39</v>
+        <v>0.17449999999999999</v>
       </c>
       <c r="O32" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2506142506142506</v>
+        <v>1.2496551724137932</v>
       </c>
       <c r="P32" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2482758620689656</v>
       </c>
       <c r="Q32" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2484076433121019</v>
+        <v>1.2517985611510791</v>
       </c>
       <c r="R32" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2580645161290323</v>
+        <v>1.25089605734767</v>
       </c>
       <c r="S32" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E33" s="27">
-        <v>0.33677000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="F33" s="27">
-        <v>0.13471</v>
+        <v>0.1</v>
       </c>
       <c r="G33" s="26">
-        <v>8.7465000000000004E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H33" s="26">
-        <v>1.7493000000000001E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I33" s="26">
-        <v>9.6469999999999998E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J33" s="26">
-        <v>2.187E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K33" s="28">
-        <v>1.6820999999999999</v>
+        <v>0.625</v>
       </c>
       <c r="L33" s="28">
-        <v>0.33639999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="M33" s="28">
-        <v>2.1025999999999998</v>
+        <v>0.78</v>
       </c>
       <c r="N33" s="28">
-        <v>0.42099999999999999</v>
+        <v>0.155</v>
       </c>
       <c r="O33" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.1029554679014462</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="P33" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2502143714628708</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="Q33" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499851376255871</v>
+        <v>1.248</v>
       </c>
       <c r="R33" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2514863258026159</v>
+        <v>1.24</v>
       </c>
       <c r="S33" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.40000593877126822</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated Cost Template default prices, for 2024 price reductions
</commit_message>
<xml_diff>
--- a/Excel/DynamoDB+Cost+Template.xlsx
+++ b/Excel/DynamoDB+Cost+Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/amazon-dynamodb-tools/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/cost/amazon-dynamodb-tools/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637BC981-68CE-E343-A4F1-CF6A946FAF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C70C34-F767-C840-BC3F-DF6E5032D8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16160" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
   </bookViews>
   <sheets>
     <sheet name="CostSheet" sheetId="5" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="212">
   <si>
     <t>Actual Storage</t>
   </si>
@@ -1785,6 +1785,114 @@
     <t>RatioOD_RCU</t>
   </si>
   <si>
+    <t>RCU</t>
+  </si>
+  <si>
+    <t>WCU</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Unit size (KB) for reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Demand price per each unit consumed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provisioned hourly pricing for a level of 1 Unit per second </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage Costs per GB-hr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time unit </t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time unit Qty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provisioning Efficiency % </t>
+  </si>
+  <si>
+    <t>Global Table?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> On Demand mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Provisioned mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Storage</t>
+  </si>
+  <si>
+    <t>Average read units per second</t>
+  </si>
+  <si>
+    <t>Read cost:</t>
+  </si>
+  <si>
+    <t>Average write units per second</t>
+  </si>
+  <si>
+    <t>Write cost:</t>
+  </si>
+  <si>
+    <t>Table size in GB</t>
+  </si>
+  <si>
+    <t>Storage cost:</t>
+  </si>
+  <si>
+    <t>Green values can be changed to adjust the cost model</t>
+  </si>
+  <si>
+    <t>DynamoDB capacity is either On Demand or Provisioned. This model shows you the cost of each, and assumes you would need to over provision somewhat, resulting in less than 100% provisioning efficiency.</t>
+  </si>
+  <si>
+    <t>**Note: Global Tables simplifies prices to 2x storage and 3x write costs compared to the single region table</t>
+  </si>
+  <si>
+    <t>Time Unit List</t>
+  </si>
+  <si>
+    <t>Global Tables</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Yes, 2 regions</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Actual Read/Write Cost($):</t>
+  </si>
+  <si>
+    <t>Actual Storage Cost($):</t>
+  </si>
+  <si>
+    <t>TotalCost($):</t>
+  </si>
+  <si>
+    <t>Yes, 3 regions</t>
+  </si>
+  <si>
+    <t>Yes, MRSC</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">DynamoDB Cost Template
 </t>
@@ -1795,110 +1903,8 @@
         <color theme="0"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>Prices in us-east-1</t>
+      <t>Prices in us-east-1, updated for 2025</t>
     </r>
-  </si>
-  <si>
-    <t>RCU</t>
-  </si>
-  <si>
-    <t>WCU</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Unit size (KB) for reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Demand price per each unit consumed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provisioned hourly pricing for a level of 1 Unit per second </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage Costs per GB-hr </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time unit </t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time unit Qty </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provisioning Efficiency % </t>
-  </si>
-  <si>
-    <t>Global Table?</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> On Demand mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Provisioned mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Storage</t>
-  </si>
-  <si>
-    <t>Average read units per second</t>
-  </si>
-  <si>
-    <t>Read cost:</t>
-  </si>
-  <si>
-    <t>Average write units per second</t>
-  </si>
-  <si>
-    <t>Write cost:</t>
-  </si>
-  <si>
-    <t>Table size in GB</t>
-  </si>
-  <si>
-    <t>Storage cost:</t>
-  </si>
-  <si>
-    <t>Green values can be changed to adjust the cost model</t>
-  </si>
-  <si>
-    <t>DynamoDB capacity is either On Demand or Provisioned. This model shows you the cost of each, and assumes you would need to over provision somewhat, resulting in less than 100% provisioning efficiency.</t>
-  </si>
-  <si>
-    <t>**Note: Global Tables simplifies prices to 2x storage and 3x write costs compared to the single region table</t>
-  </si>
-  <si>
-    <t>Time Unit List</t>
-  </si>
-  <si>
-    <t>Global Tables</t>
-  </si>
-  <si>
-    <t>Hour</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Yes, 2 regions</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Actual Read/Write Cost($):</t>
-  </si>
-  <si>
-    <t>Actual Storage Cost($):</t>
-  </si>
-  <si>
-    <t>TotalCost($):</t>
   </si>
 </sst>
 </file>
@@ -3786,6 +3792,96 @@
     <xf numFmtId="165" fontId="29" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3834,151 +3930,61 @@
     <xf numFmtId="164" fontId="14" fillId="6" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6676,10 +6682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A5111F-7B7D-344C-A811-3E0902529217}">
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6696,21 +6702,21 @@
     <row r="1" spans="2:7" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" s="84" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="B2" s="81" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="D2" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="E2" s="83" t="s">
         <v>177</v>
-      </c>
-      <c r="E2" s="83" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C3" s="86">
         <v>4</v>
@@ -6722,21 +6728,21 @@
     </row>
     <row r="4" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="85" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="88">
-        <f>0.25/1000000</f>
-        <v>2.4999999999999999E-7</v>
+        <f>0.125/1000000</f>
+        <v>1.2499999999999999E-7</v>
       </c>
       <c r="D4" s="88">
-        <f>1.25/1000000</f>
-        <v>1.2500000000000001E-6</v>
+        <f>0.625/1000000</f>
+        <v>6.2500000000000005E-7</v>
       </c>
       <c r="E4" s="87"/>
     </row>
     <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" s="89">
         <v>1.2999999999999999E-4</v>
@@ -6751,7 +6757,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="85" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="90"/>
       <c r="D7" s="90"/>
@@ -6761,15 +6767,15 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="93" t="s">
         <v>183</v>
-      </c>
-      <c r="C9" s="93" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="92" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" s="93">
         <v>1</v>
@@ -6781,7 +6787,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="92" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="95">
         <v>50</v>
@@ -6789,17 +6795,17 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="92" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="93" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="93" t="s">
-        <v>188</v>
-      </c>
       <c r="E12" s="94">
-        <f>_xlfn.SWITCH(GT, "No", 1, "Yes, 2 regions", 2)</f>
+        <f>_xlfn.SWITCH(GT, "No", 1, "Yes, 2 regions", 2, "Yes, 3 regions", 3, "Yes, MRSC", 3)</f>
         <v>1</v>
       </c>
       <c r="F12" s="94">
-        <f>_xlfn.SWITCH(GT, "No", 1, "Yes, 2 regions", 3)</f>
+        <f>_xlfn.SWITCH(GT, "No", 1, "Yes, 2 regions", 2, "Yes, 3 regions", 3, "Yes, MRSC", 3)</f>
         <v>1</v>
       </c>
     </row>
@@ -6814,28 +6820,28 @@
     </row>
     <row r="15" spans="2:7" s="96" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="E15" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="F15" s="100" t="s">
+      <c r="G15" s="101" t="s">
         <v>190</v>
-      </c>
-      <c r="G15" s="101" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="102" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="103">
         <v>100</v>
       </c>
       <c r="D16" s="104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16" s="105">
         <f>C16*OnDemandRcuPrice*3600*Hours</f>
-        <v>64.8</v>
+        <v>32.4</v>
       </c>
       <c r="F16" s="106">
         <f>C16*ProvisionedPricePerReadUnitHourly*Hours*(1/(ProvisioningEfficiency/100))</f>
@@ -6845,17 +6851,17 @@
     </row>
     <row r="17" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" s="103">
         <v>100</v>
       </c>
       <c r="D17" s="104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="108">
         <f>C17*OnDemandWcuPrice*3600*Hours*GTWrites</f>
-        <v>324</v>
+        <v>162</v>
       </c>
       <c r="F17" s="109">
         <f>C17*ProvisionedPricePerWriteUnitHourly*Hours*(1/(ProvisioningEfficiency/100))*GTWrites</f>
@@ -6865,13 +6871,13 @@
     </row>
     <row r="18" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C18" s="103">
         <v>100</v>
       </c>
       <c r="D18" s="104" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E18" s="107"/>
       <c r="F18" s="107"/>
@@ -6882,69 +6888,70 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="110" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="110" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="110" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>201</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>203</v>
       </c>
-      <c r="C28" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>204</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="33" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="34" hidden="1" x14ac:dyDescent="0.2"/>
+      <c r="C31" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{EA6DDBB6-4213-C942-AEE9-964048E9D090}">
-      <formula1>$C$28:$C$29</formula1>
-    </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{D6E42FBD-5461-444E-81E0-C34F8E03CE7D}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{002149AF-C7EA-E945-B9C4-26D82F61BFEA}">
       <formula1>$B$28:$B$31</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{EA6DDBB6-4213-C942-AEE9-964048E9D090}">
+      <formula1>$C$28:$C$31</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6958,8 +6965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE6116E-4397-EA44-966F-6DDC633C7C56}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="G9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6999,32 +7006,32 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="156"/>
-      <c r="G3" s="122" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
+      <c r="G3" s="152" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
     </row>
     <row r="4" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="157" t="s">
+      <c r="C4" s="134"/>
+      <c r="D4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="126"/>
       <c r="G4" s="41" t="s">
         <v>135</v>
       </c>
@@ -7039,15 +7046,15 @@
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="148">
+      <c r="B5" s="135">
         <v>1000</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="159" cm="1">
+      <c r="C5" s="136"/>
+      <c r="D5" s="127" cm="1">
         <f t="array" ref="D5">_xlfn.IFS(H4="Provisioned capacity",B5*I36,H4="On Demand",B5*M36)</f>
         <v>1251.0204081632655</v>
       </c>
-      <c r="E5" s="160"/>
+      <c r="E5" s="128"/>
       <c r="G5" s="41" t="s">
         <v>134</v>
       </c>
@@ -7063,15 +7070,15 @@
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="164">
+      <c r="B6" s="137">
         <v>100</v>
       </c>
-      <c r="C6" s="165"/>
-      <c r="D6" s="161">
+      <c r="C6" s="138"/>
+      <c r="D6" s="129">
         <f>B6*P36</f>
         <v>40</v>
       </c>
-      <c r="E6" s="143"/>
+      <c r="E6" s="130"/>
       <c r="G6" s="42" t="s">
         <v>131</v>
       </c>
@@ -7087,16 +7094,16 @@
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="166">
+      <c r="B7" s="139">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="167"/>
-      <c r="D7" s="162">
+      <c r="C7" s="140"/>
+      <c r="D7" s="131">
         <f>SUM(D5:D6)</f>
         <v>1291.0204081632655</v>
       </c>
-      <c r="E7" s="163"/>
+      <c r="E7" s="132"/>
       <c r="G7" s="37"/>
       <c r="H7" s="74" t="s">
         <v>122</v>
@@ -7236,13 +7243,13 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="155"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="156"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
       <c r="G15" s="43" t="s">
         <v>124</v>
       </c>
@@ -7266,14 +7273,14 @@
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="147"/>
-      <c r="D16" s="138" t="s">
+      <c r="C16" s="134"/>
+      <c r="D16" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="139"/>
+      <c r="E16" s="142"/>
       <c r="G16" s="46" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.IFS($H$4="On Demand", "RRU", $H$4="Provisioned Capacity", "RCU")</f>
         <v>RCU</v>
@@ -7290,11 +7297,11 @@
         <f t="array" ref="J16">_xlfn.IFS($H$4="Provisioned Capacity",$I$16*$H$30,$H$4="On Demand",$I$16*$L$30/1000000)</f>
         <v>7.665</v>
       </c>
-      <c r="K16" s="136">
+      <c r="K16" s="166">
         <f>$J$16+$J$17</f>
         <v>160.965</v>
       </c>
-      <c r="L16" s="130">
+      <c r="L16" s="160">
         <f>$K$16+$K$18</f>
         <v>160.965</v>
       </c>
@@ -7303,15 +7310,15 @@
       <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="148">
+      <c r="B17" s="135">
         <v>1251</v>
       </c>
-      <c r="C17" s="149"/>
-      <c r="D17" s="140" cm="1">
+      <c r="C17" s="136"/>
+      <c r="D17" s="143" cm="1">
         <f t="array" ref="D17">_xlfn.IFS(H4="Provisioned capacity",B17/I36,H4="On Demand",B17/M36)</f>
         <v>999.98368678629686</v>
       </c>
-      <c r="E17" s="141"/>
+      <c r="E17" s="144"/>
       <c r="G17" s="47" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.IFS($H$4="On Demand", "WRU", $H$4="Provisioned Capacity", "WCU")</f>
         <v>WCU</v>
@@ -7328,51 +7335,51 @@
         <f t="array" ref="J17">_xlfn.IFS($H$4="Provisioned Capacity",$I$17*$G$30,$H$4="On Demand",$I$17*$K$30/1000000)</f>
         <v>153.30000000000001</v>
       </c>
-      <c r="K17" s="137"/>
-      <c r="L17" s="131"/>
+      <c r="K17" s="167"/>
+      <c r="L17" s="161"/>
     </row>
     <row r="18" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="150">
+      <c r="B18" s="148">
         <v>200</v>
       </c>
-      <c r="C18" s="151"/>
-      <c r="D18" s="142">
+      <c r="C18" s="149"/>
+      <c r="D18" s="145">
         <f>B18/P36</f>
         <v>500</v>
       </c>
-      <c r="E18" s="143"/>
+      <c r="E18" s="130"/>
       <c r="G18" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="125">
+      <c r="H18" s="155">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="126"/>
-      <c r="J18" s="127"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="157"/>
       <c r="K18" s="45">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="132"/>
+      <c r="L18" s="162"/>
     </row>
     <row r="19" spans="1:16" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="152">
+      <c r="B19" s="150">
         <f>SUM(B17:B18)</f>
         <v>1451</v>
       </c>
-      <c r="C19" s="153"/>
-      <c r="D19" s="144">
+      <c r="C19" s="151"/>
+      <c r="D19" s="146">
         <f>SUM(D17:D18)</f>
         <v>1499.9836867862969</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="147"/>
       <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7449,11 +7456,11 @@
         <f t="array" ref="J21">_xlfn.IFS($H$4="Provisioned Capacity",$I$21*$J$30,$H$4="On Demand",$I$21*$N$30/1000000)</f>
         <v>9.5942857142857143</v>
       </c>
-      <c r="K21" s="136">
+      <c r="K21" s="166">
         <f>$J$21+$J$22</f>
         <v>201.27142857142857</v>
       </c>
-      <c r="L21" s="133">
+      <c r="L21" s="163">
         <f>$K$21+$K$23</f>
         <v>201.27142857142857</v>
       </c>
@@ -7481,24 +7488,24 @@
         <f t="array" ref="J22">_xlfn.IFS($H$4="Provisioned Capacity",$I$22*$I$30,$H$4="On Demand",$I$22*$M$30/1000000)</f>
         <v>191.67714285714285</v>
       </c>
-      <c r="K22" s="137"/>
-      <c r="L22" s="134"/>
+      <c r="K22" s="167"/>
+      <c r="L22" s="164"/>
     </row>
     <row r="23" spans="1:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="H23" s="128">
+      <c r="H23" s="158">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="126"/>
-      <c r="J23" s="127"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="45">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="135"/>
+      <c r="L23" s="165"/>
     </row>
     <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -7629,19 +7636,19 @@
       <c r="H36" t="s">
         <v>132</v>
       </c>
-      <c r="I36" s="129">
+      <c r="I36" s="159">
         <f>$J$35*($H$11/($H$11+$H$12))+$I$35*($H$12/($H$12+$H$11))</f>
         <v>1.2510204081632654</v>
       </c>
-      <c r="J36" s="129"/>
+      <c r="J36" s="159"/>
       <c r="L36" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="129">
+      <c r="M36" s="159">
         <f>$N$35*($H$11/($H$11+$H$12))+$M$35*($H$12/($H$12+$H$11))</f>
         <v>1.2504505394098553</v>
       </c>
-      <c r="N36" s="129"/>
+      <c r="N36" s="159"/>
       <c r="P36">
         <f>$P$30/$O$30</f>
         <v>0.4</v>
@@ -7652,6 +7659,23 @@
     <row r="40" spans="8:16" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -7662,23 +7686,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K16:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="lessThan">
@@ -7806,67 +7813,67 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="156"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
     </row>
     <row r="4" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="186"/>
-      <c r="D4" s="157" t="s">
+      <c r="C4" s="172"/>
+      <c r="D4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" s="183">
+        <v>206</v>
+      </c>
+      <c r="B5" s="168">
         <v>1000</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="185">
+      <c r="C5" s="169"/>
+      <c r="D5" s="170">
         <f>B5*1.25</f>
         <v>1250</v>
       </c>
-      <c r="E5" s="160"/>
+      <c r="E5" s="128"/>
     </row>
     <row r="6" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" s="177">
+        <v>207</v>
+      </c>
+      <c r="B6" s="179">
         <v>100</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179">
+      <c r="C6" s="180"/>
+      <c r="D6" s="181">
         <f>B6*0.4</f>
         <v>40</v>
       </c>
-      <c r="E6" s="180"/>
+      <c r="E6" s="182"/>
     </row>
     <row r="7" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="B7" s="174">
+        <v>208</v>
+      </c>
+      <c r="B7" s="176">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="175"/>
-      <c r="D7" s="181">
+      <c r="C7" s="177"/>
+      <c r="D7" s="183">
         <f>SUM(D5:D6)</f>
         <v>1290</v>
       </c>
-      <c r="E7" s="182"/>
+      <c r="E7" s="184"/>
     </row>
     <row r="8" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -7949,67 +7956,67 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="155"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="156"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
     </row>
     <row r="16" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="168" t="s">
+      <c r="C16" s="141"/>
+      <c r="D16" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="139"/>
+      <c r="E16" s="142"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="169">
+      <c r="B17" s="185">
         <v>6000</v>
       </c>
-      <c r="C17" s="170"/>
-      <c r="D17" s="159">
+      <c r="C17" s="186"/>
+      <c r="D17" s="127">
         <f>B17/1.25</f>
         <v>4800</v>
       </c>
-      <c r="E17" s="160"/>
+      <c r="E17" s="128"/>
     </row>
     <row r="18" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="171">
+      <c r="B18" s="173">
         <v>168</v>
       </c>
-      <c r="C18" s="172"/>
-      <c r="D18" s="173">
+      <c r="C18" s="174"/>
+      <c r="D18" s="175">
         <f>B18/0.4</f>
         <v>420</v>
       </c>
-      <c r="E18" s="143"/>
+      <c r="E18" s="130"/>
     </row>
     <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="174">
+      <c r="B19" s="176">
         <f>SUM(B17:B18)</f>
         <v>6168</v>
       </c>
-      <c r="C19" s="175"/>
-      <c r="D19" s="176">
+      <c r="C19" s="177"/>
+      <c r="D19" s="178">
         <f>SUM(D17:D18)</f>
         <v>5220</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="147"/>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
@@ -8065,11 +8072,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B19:C19"/>
@@ -8083,6 +8085,11 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="lessThan">

</xml_diff>

<commit_message>
updated Cost Template default prices, with 2024 price reductions
</commit_message>
<xml_diff>
--- a/Excel/DynamoDB+Cost+Template.xlsx
+++ b/Excel/DynamoDB+Cost+Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/cost/amazon-dynamodb-tools/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C70C34-F767-C840-BC3F-DF6E5032D8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A5D268E-5257-CB4D-89F3-240A0D5E53B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16160" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
   </bookViews>
   <sheets>
     <sheet name="CostSheet" sheetId="5" r:id="rId1"/>
@@ -3792,6 +3792,102 @@
     <xf numFmtId="165" fontId="29" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="69" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="70" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="56" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3816,27 +3912,12 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3849,86 +3930,50 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="69" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="70" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="56" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3939,52 +3984,7 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6684,8 +6684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A5111F-7B7D-344C-A811-3E0902529217}">
   <dimension ref="B1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6901,7 +6901,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>200</v>
       </c>
@@ -6909,7 +6910,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>202</v>
       </c>
@@ -6917,7 +6918,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>203</v>
       </c>
@@ -6925,7 +6926,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>183</v>
       </c>
@@ -6933,7 +6934,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>205</v>
       </c>
@@ -7006,32 +7007,32 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="124"/>
-      <c r="G3" s="152" t="s">
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="156"/>
+      <c r="G3" s="122" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="154"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
     </row>
     <row r="4" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="125" t="s">
+      <c r="C4" s="147"/>
+      <c r="D4" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="126"/>
+      <c r="E4" s="158"/>
       <c r="G4" s="41" t="s">
         <v>135</v>
       </c>
@@ -7046,15 +7047,15 @@
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="135">
+      <c r="B5" s="148">
         <v>1000</v>
       </c>
-      <c r="C5" s="136"/>
-      <c r="D5" s="127" cm="1">
+      <c r="C5" s="149"/>
+      <c r="D5" s="159" cm="1">
         <f t="array" ref="D5">_xlfn.IFS(H4="Provisioned capacity",B5*I36,H4="On Demand",B5*M36)</f>
         <v>1251.0204081632655</v>
       </c>
-      <c r="E5" s="128"/>
+      <c r="E5" s="160"/>
       <c r="G5" s="41" t="s">
         <v>134</v>
       </c>
@@ -7070,15 +7071,15 @@
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="137">
+      <c r="B6" s="164">
         <v>100</v>
       </c>
-      <c r="C6" s="138"/>
-      <c r="D6" s="129">
+      <c r="C6" s="165"/>
+      <c r="D6" s="161">
         <f>B6*P36</f>
         <v>40</v>
       </c>
-      <c r="E6" s="130"/>
+      <c r="E6" s="143"/>
       <c r="G6" s="42" t="s">
         <v>131</v>
       </c>
@@ -7094,16 +7095,16 @@
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="139">
+      <c r="B7" s="166">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="140"/>
-      <c r="D7" s="131">
+      <c r="C7" s="167"/>
+      <c r="D7" s="162">
         <f>SUM(D5:D6)</f>
         <v>1291.0204081632655</v>
       </c>
-      <c r="E7" s="132"/>
+      <c r="E7" s="163"/>
       <c r="G7" s="37"/>
       <c r="H7" s="74" t="s">
         <v>122</v>
@@ -7243,13 +7244,13 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="124"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="156"/>
       <c r="G15" s="43" t="s">
         <v>124</v>
       </c>
@@ -7273,14 +7274,14 @@
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="133" t="s">
+      <c r="B16" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="134"/>
-      <c r="D16" s="141" t="s">
+      <c r="C16" s="147"/>
+      <c r="D16" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="142"/>
+      <c r="E16" s="139"/>
       <c r="G16" s="46" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.IFS($H$4="On Demand", "RRU", $H$4="Provisioned Capacity", "RCU")</f>
         <v>RCU</v>
@@ -7297,11 +7298,11 @@
         <f t="array" ref="J16">_xlfn.IFS($H$4="Provisioned Capacity",$I$16*$H$30,$H$4="On Demand",$I$16*$L$30/1000000)</f>
         <v>7.665</v>
       </c>
-      <c r="K16" s="166">
+      <c r="K16" s="136">
         <f>$J$16+$J$17</f>
         <v>160.965</v>
       </c>
-      <c r="L16" s="160">
+      <c r="L16" s="130">
         <f>$K$16+$K$18</f>
         <v>160.965</v>
       </c>
@@ -7310,15 +7311,15 @@
       <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="135">
+      <c r="B17" s="148">
         <v>1251</v>
       </c>
-      <c r="C17" s="136"/>
-      <c r="D17" s="143" cm="1">
+      <c r="C17" s="149"/>
+      <c r="D17" s="140" cm="1">
         <f t="array" ref="D17">_xlfn.IFS(H4="Provisioned capacity",B17/I36,H4="On Demand",B17/M36)</f>
         <v>999.98368678629686</v>
       </c>
-      <c r="E17" s="144"/>
+      <c r="E17" s="141"/>
       <c r="G17" s="47" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.IFS($H$4="On Demand", "WRU", $H$4="Provisioned Capacity", "WCU")</f>
         <v>WCU</v>
@@ -7335,51 +7336,51 @@
         <f t="array" ref="J17">_xlfn.IFS($H$4="Provisioned Capacity",$I$17*$G$30,$H$4="On Demand",$I$17*$K$30/1000000)</f>
         <v>153.30000000000001</v>
       </c>
-      <c r="K17" s="167"/>
-      <c r="L17" s="161"/>
+      <c r="K17" s="137"/>
+      <c r="L17" s="131"/>
     </row>
     <row r="18" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="148">
+      <c r="B18" s="150">
         <v>200</v>
       </c>
-      <c r="C18" s="149"/>
-      <c r="D18" s="145">
+      <c r="C18" s="151"/>
+      <c r="D18" s="142">
         <f>B18/P36</f>
         <v>500</v>
       </c>
-      <c r="E18" s="130"/>
+      <c r="E18" s="143"/>
       <c r="G18" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="155">
+      <c r="H18" s="125">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="156"/>
-      <c r="J18" s="157"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="127"/>
       <c r="K18" s="45">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="162"/>
+      <c r="L18" s="132"/>
     </row>
     <row r="19" spans="1:16" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="150">
+      <c r="B19" s="152">
         <f>SUM(B17:B18)</f>
         <v>1451</v>
       </c>
-      <c r="C19" s="151"/>
-      <c r="D19" s="146">
+      <c r="C19" s="153"/>
+      <c r="D19" s="144">
         <f>SUM(D17:D18)</f>
         <v>1499.9836867862969</v>
       </c>
-      <c r="E19" s="147"/>
+      <c r="E19" s="145"/>
       <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7456,11 +7457,11 @@
         <f t="array" ref="J21">_xlfn.IFS($H$4="Provisioned Capacity",$I$21*$J$30,$H$4="On Demand",$I$21*$N$30/1000000)</f>
         <v>9.5942857142857143</v>
       </c>
-      <c r="K21" s="166">
+      <c r="K21" s="136">
         <f>$J$21+$J$22</f>
         <v>201.27142857142857</v>
       </c>
-      <c r="L21" s="163">
+      <c r="L21" s="133">
         <f>$K$21+$K$23</f>
         <v>201.27142857142857</v>
       </c>
@@ -7488,24 +7489,24 @@
         <f t="array" ref="J22">_xlfn.IFS($H$4="Provisioned Capacity",$I$22*$I$30,$H$4="On Demand",$I$22*$M$30/1000000)</f>
         <v>191.67714285714285</v>
       </c>
-      <c r="K22" s="167"/>
-      <c r="L22" s="164"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="134"/>
     </row>
     <row r="23" spans="1:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="H23" s="158">
+      <c r="H23" s="128">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="156"/>
-      <c r="J23" s="157"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="127"/>
       <c r="K23" s="45">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="165"/>
+      <c r="L23" s="135"/>
     </row>
     <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -7636,19 +7637,19 @@
       <c r="H36" t="s">
         <v>132</v>
       </c>
-      <c r="I36" s="159">
+      <c r="I36" s="129">
         <f>$J$35*($H$11/($H$11+$H$12))+$I$35*($H$12/($H$12+$H$11))</f>
         <v>1.2510204081632654</v>
       </c>
-      <c r="J36" s="159"/>
+      <c r="J36" s="129"/>
       <c r="L36" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="159">
+      <c r="M36" s="129">
         <f>$N$35*($H$11/($H$11+$H$12))+$M$35*($H$12/($H$12+$H$11))</f>
         <v>1.2504505394098553</v>
       </c>
-      <c r="N36" s="159"/>
+      <c r="N36" s="129"/>
       <c r="P36">
         <f>$P$30/$O$30</f>
         <v>0.4</v>
@@ -7659,23 +7660,6 @@
     <row r="40" spans="8:16" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -7686,6 +7670,23 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K16:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="lessThan">
@@ -7813,67 +7814,67 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="124"/>
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="156"/>
     </row>
     <row r="4" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="180" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="125" t="s">
+      <c r="C4" s="186"/>
+      <c r="D4" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="126"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="168">
+      <c r="B5" s="183">
         <v>1000</v>
       </c>
-      <c r="C5" s="169"/>
-      <c r="D5" s="170">
+      <c r="C5" s="184"/>
+      <c r="D5" s="185">
         <f>B5*1.25</f>
         <v>1250</v>
       </c>
-      <c r="E5" s="128"/>
+      <c r="E5" s="160"/>
     </row>
     <row r="6" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="179">
+      <c r="B6" s="174">
         <v>100</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181">
+      <c r="C6" s="175"/>
+      <c r="D6" s="176">
         <f>B6*0.4</f>
         <v>40</v>
       </c>
-      <c r="E6" s="182"/>
+      <c r="E6" s="177"/>
     </row>
     <row r="7" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="176">
+      <c r="B7" s="171">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="177"/>
-      <c r="D7" s="183">
+      <c r="C7" s="172"/>
+      <c r="D7" s="178">
         <f>SUM(D5:D6)</f>
         <v>1290</v>
       </c>
-      <c r="E7" s="184"/>
+      <c r="E7" s="179"/>
     </row>
     <row r="8" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -7956,67 +7957,67 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="124"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="156"/>
     </row>
     <row r="16" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="141"/>
-      <c r="D16" s="171" t="s">
+      <c r="C16" s="138"/>
+      <c r="D16" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="142"/>
+      <c r="E16" s="139"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="185">
+      <c r="B17" s="181">
         <v>6000</v>
       </c>
-      <c r="C17" s="186"/>
-      <c r="D17" s="127">
+      <c r="C17" s="182"/>
+      <c r="D17" s="159">
         <f>B17/1.25</f>
         <v>4800</v>
       </c>
-      <c r="E17" s="128"/>
+      <c r="E17" s="160"/>
     </row>
     <row r="18" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="173">
+      <c r="B18" s="168">
         <v>168</v>
       </c>
-      <c r="C18" s="174"/>
-      <c r="D18" s="175">
+      <c r="C18" s="169"/>
+      <c r="D18" s="170">
         <f>B18/0.4</f>
         <v>420</v>
       </c>
-      <c r="E18" s="130"/>
+      <c r="E18" s="143"/>
     </row>
     <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="176">
+      <c r="B19" s="171">
         <f>SUM(B17:B18)</f>
         <v>6168</v>
       </c>
-      <c r="C19" s="177"/>
-      <c r="D19" s="178">
+      <c r="C19" s="172"/>
+      <c r="D19" s="173">
         <f>SUM(D17:D18)</f>
         <v>5220</v>
       </c>
-      <c r="E19" s="147"/>
+      <c r="E19" s="145"/>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
@@ -8072,6 +8073,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B19:C19"/>
@@ -8085,11 +8091,6 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="lessThan">

</xml_diff>

<commit_message>
Excel cost calculator, all sheets updated for new prices
</commit_message>
<xml_diff>
--- a/Excel/DynamoDB+Cost+Template.xlsx
+++ b/Excel/DynamoDB+Cost+Template.xlsx
@@ -5,33 +5,45 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/cost/amazon-dynamodb-tools/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccaul/Projects/scratch/amazon-dynamodb-tools/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A5D268E-5257-CB4D-89F3-240A0D5E53B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75131595-A095-0543-9C7F-E2CC6B6C0627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
+    <workbookView xWindow="-1700" yWindow="-20880" windowWidth="23820" windowHeight="16640" xr2:uid="{8F366F91-9D43-B54C-80F1-BE22DE501760}"/>
   </bookViews>
   <sheets>
-    <sheet name="CostSheet" sheetId="5" r:id="rId1"/>
+    <sheet name="CostSheet" sheetId="7" r:id="rId1"/>
     <sheet name="Table Class Calc (Cost Unknown)" sheetId="2" r:id="rId2"/>
     <sheet name="Table Class Calc(Cost Known)" sheetId="6" r:id="rId3"/>
     <sheet name="Data" sheetId="3" state="hidden" r:id="rId4"/>
     <sheet name="List" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="GT">CostSheet!$C$12</definedName>
-    <definedName name="GTStorage">CostSheet!$E$12</definedName>
-    <definedName name="GTWrites">CostSheet!$F$12</definedName>
-    <definedName name="Hours">CostSheet!$E$10</definedName>
-    <definedName name="OnDemandRcuPrice">CostSheet!$C$4</definedName>
-    <definedName name="OnDemandWcuPrice">CostSheet!$D$4</definedName>
-    <definedName name="ProvisionedPricePerReadUnitHourly">CostSheet!$C$5</definedName>
-    <definedName name="ProvisionedPricePerWriteUnitHourly">CostSheet!$D$5</definedName>
-    <definedName name="ProvisioningEfficiency">CostSheet!$C$11</definedName>
-    <definedName name="StorageCostPerGbHour">CostSheet!$E$7</definedName>
-    <definedName name="TimeUnit">CostSheet!$C$9</definedName>
-    <definedName name="TimeUnitQty">CostSheet!$C$10</definedName>
+    <definedName name="GT" localSheetId="0">CostSheet!$C$12</definedName>
+    <definedName name="GT">#REF!</definedName>
+    <definedName name="GTStorage" localSheetId="0">CostSheet!$E$12</definedName>
+    <definedName name="GTStorage">#REF!</definedName>
+    <definedName name="GTWrites" localSheetId="0">CostSheet!$F$12</definedName>
+    <definedName name="GTWrites">#REF!</definedName>
+    <definedName name="Hours" localSheetId="0">CostSheet!$E$10</definedName>
+    <definedName name="Hours">#REF!</definedName>
+    <definedName name="OnDemandRcuPrice" localSheetId="0">CostSheet!$C$4</definedName>
+    <definedName name="OnDemandRcuPrice">#REF!</definedName>
+    <definedName name="OnDemandWcuPrice" localSheetId="0">CostSheet!$D$4</definedName>
+    <definedName name="OnDemandWcuPrice">#REF!</definedName>
+    <definedName name="ProvisionedPricePerReadUnitHourly" localSheetId="0">CostSheet!$C$5</definedName>
+    <definedName name="ProvisionedPricePerReadUnitHourly">#REF!</definedName>
+    <definedName name="ProvisionedPricePerWriteUnitHourly" localSheetId="0">CostSheet!$D$5</definedName>
+    <definedName name="ProvisionedPricePerWriteUnitHourly">#REF!</definedName>
+    <definedName name="ProvisioningEfficiency" localSheetId="0">CostSheet!$C$11</definedName>
+    <definedName name="ProvisioningEfficiency">#REF!</definedName>
+    <definedName name="StorageCostPerGbHour" localSheetId="0">CostSheet!$E$7</definedName>
+    <definedName name="StorageCostPerGbHour">#REF!</definedName>
+    <definedName name="TimeUnit" localSheetId="0">CostSheet!$C$9</definedName>
+    <definedName name="TimeUnit">#REF!</definedName>
+    <definedName name="TimeUnitQty" localSheetId="0">CostSheet!$C$10</definedName>
+    <definedName name="TimeUnitQty">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -138,7 +150,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Provisiond Capacity:</t>
         </r>
@@ -148,7 +159,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -159,49 +169,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Your Auto Scaling</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>target utilization (use 100% if AutoScaling</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> is disabled)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Your Auto Scaling target utilization (use 100% if AutoScaling is disabled)
 </t>
         </r>
         <r>
@@ -210,9 +179,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t xml:space="preserve">0%-100%.
+          <t xml:space="preserve">20%-90%.
 </t>
         </r>
         <r>
@@ -221,7 +189,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The default is 70%.
 </t>
@@ -232,7 +199,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">For example, if you choose 70% of your total capacity, it will add a buffer of 30% of your throughput to handle spikes. This implies that if you select 70 strongly consistent reads per second, the calculation will assume 100 strongly consistent reads per second (100 RCUs). 
 </t>
@@ -243,7 +209,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The higher the percentage you choose, the lower your cost will be. 
 </t>
@@ -254,7 +219,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -266,7 +230,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>On-Demand:</t>
         </r>
@@ -276,7 +239,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -287,7 +249,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The calculation determines the average percentage of the monthly capacity. For example, if you choose 50% and 100 strongly consistent reads per second, the calculation will assume you are requesting 50 requests per second for the entire month (50x3600cx730 = 131.4M requests per month).
 </t>
@@ -298,7 +259,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -309,7 +269,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">As a general rule, your utilization should be less than 18% of the provisioned capacity when using on-demand to save costs.
 </t>
@@ -320,7 +279,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -331,7 +289,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The higher the percentage you choose, the higher your cost will be. 
 </t>
@@ -342,7 +299,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t> </t>
         </r>
@@ -518,7 +474,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The sum of the percentage of eventual cosistancy, strong consistancy, and transaction reads </t>
         </r>
@@ -529,7 +484,6 @@
             <color rgb="FFFF0000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">must be equal to 100%. </t>
         </r>
@@ -539,7 +493,6 @@
             <color rgb="FFFF0000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -550,7 +503,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The default is 100% eventual consistency.</t>
         </r>
@@ -1887,10 +1839,10 @@
     <t>TotalCost($):</t>
   </si>
   <si>
+    <t>Yes, MRSC</t>
+  </si>
+  <si>
     <t>Yes, 3 regions</t>
-  </si>
-  <si>
-    <t>Yes, MRSC</t>
   </si>
   <si>
     <r>
@@ -2201,21 +2153,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2331,6 +2268,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3701,56 +3651,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="173" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="49" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="173" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="51" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -3765,22 +3715,22 @@
     <xf numFmtId="2" fontId="12" fillId="5" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="53" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="51" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3792,6 +3742,96 @@
     <xf numFmtId="165" fontId="29" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3840,100 +3880,25 @@
     <xf numFmtId="164" fontId="14" fillId="6" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3948,10 +3913,10 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3966,25 +3931,10 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6334,7 +6284,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7061F7D0-B36B-DD47-8C46-CF821975800D}" name="Table1" displayName="Table1" ref="B27:C31" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE38CED7-8211-4242-8B30-5C555DF4CA49}" name="Table1" displayName="Table1" ref="B27:C31" totalsRowShown="0">
   <autoFilter ref="B27:C31" xr:uid="{7061F7D0-B36B-DD47-8C46-CF821975800D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B443148E-431E-ED46-84E0-B842F4959136}" name="Time Unit List"/>
@@ -6347,8 +6297,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D6EA7312-83FB-3648-A8CB-C88F5565BFA1}" name="Table4" displayName="Table4" ref="A2:S34" totalsRowCount="1">
   <autoFilter ref="A2:S33" xr:uid="{D6EA7312-83FB-3648-A8CB-C88F5565BFA1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N33">
-    <sortCondition descending="1" ref="A2:A33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:S33">
+    <sortCondition ref="D2:D33"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{4F795EE2-B6FB-B742-8C31-9011902642B6}" name="# aws_region"/>
@@ -6681,11 +6631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A5111F-7B7D-344C-A811-3E0902529217}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75ACE45-4735-AF43-8002-FA199D994036}">
   <dimension ref="B1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6931,7 +6881,7 @@
         <v>183</v>
       </c>
       <c r="C30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="2:7" hidden="1" x14ac:dyDescent="0.2">
@@ -6939,20 +6889,20 @@
         <v>205</v>
       </c>
       <c r="C31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{D6E42FBD-5461-444E-81E0-C34F8E03CE7D}">
-      <formula1>1</formula1>
-      <formula2>100</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{EA6DDBB6-4213-C942-AEE9-964048E9D090}">
+      <formula1>$C$28:$C$31</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{002149AF-C7EA-E945-B9C4-26D82F61BFEA}">
       <formula1>$B$28:$B$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{EA6DDBB6-4213-C942-AEE9-964048E9D090}">
-      <formula1>$C$28:$C$31</formula1>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{D6E42FBD-5461-444E-81E0-C34F8E03CE7D}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6966,8 +6916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE6116E-4397-EA44-966F-6DDC633C7C56}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7007,104 +6957,104 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="156"/>
-      <c r="G3" s="122" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
+      <c r="G3" s="152" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
     </row>
     <row r="4" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="157" t="s">
+      <c r="C4" s="134"/>
+      <c r="D4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="126"/>
       <c r="G4" s="41" t="s">
         <v>135</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I4" s="73">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="148">
+      <c r="B5" s="135">
         <v>1000</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="159" cm="1">
+      <c r="C5" s="136"/>
+      <c r="D5" s="127" cm="1">
         <f t="array" ref="D5">_xlfn.IFS(H4="Provisioned capacity",B5*I36,H4="On Demand",B5*M36)</f>
-        <v>1251.0204081632655</v>
-      </c>
-      <c r="E5" s="160"/>
+        <v>1240</v>
+      </c>
+      <c r="E5" s="128"/>
       <c r="G5" s="41" t="s">
         <v>134</v>
       </c>
       <c r="H5" s="70" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="I5" s="71" t="str">
         <f>VLOOKUP(H5,Table4[[#All],['# aws_region]:[city]],4,0)</f>
-        <v>Europe (Ireland)</v>
+        <v>US East (N. Virginia)</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="164">
+      <c r="B6" s="137">
         <v>100</v>
       </c>
-      <c r="C6" s="165"/>
-      <c r="D6" s="161">
+      <c r="C6" s="138"/>
+      <c r="D6" s="129">
         <f>B6*P36</f>
         <v>40</v>
       </c>
-      <c r="E6" s="143"/>
+      <c r="E6" s="130"/>
       <c r="G6" s="42" t="s">
         <v>131</v>
       </c>
       <c r="H6" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="59" t="str">
         <f>H6*1024&amp;(" Bytes")</f>
-        <v>2048 Bytes</v>
+        <v>1024 Bytes</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="166">
+      <c r="B7" s="139">
         <f>SUM(B5:B6)</f>
         <v>1100</v>
       </c>
-      <c r="C7" s="167"/>
-      <c r="D7" s="162">
+      <c r="C7" s="140"/>
+      <c r="D7" s="131">
         <f>SUM(D5:D6)</f>
-        <v>1291.0204081632655</v>
-      </c>
-      <c r="E7" s="163"/>
+        <v>1280</v>
+      </c>
+      <c r="E7" s="132"/>
       <c r="G7" s="37"/>
       <c r="H7" s="74" t="s">
         <v>122</v>
@@ -7159,7 +7109,7 @@
       </c>
       <c r="E9" s="17" cm="1">
         <f t="array" ref="E9">_xlfn.IFS(H4="Provisioned capacity",(1-P36)*B6 - (I36-1)*B5,H4="On Demand",(1-P36)*B6 - (M36-1)*B5)</f>
-        <v>-191.02040816326542</v>
+        <v>-180</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="41" t="s">
@@ -7202,7 +7152,7 @@
         <v>128</v>
       </c>
       <c r="H11" s="55">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="I11" s="57"/>
       <c r="K11" s="2"/>
@@ -7217,7 +7167,7 @@
         <v>129</v>
       </c>
       <c r="H12" s="60">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I12" s="58"/>
     </row>
@@ -7231,7 +7181,7 @@
         <v>130</v>
       </c>
       <c r="H13" s="56">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I13" s="59"/>
     </row>
@@ -7244,23 +7194,23 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="155"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="156"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
       <c r="G15" s="43" t="s">
         <v>124</v>
       </c>
       <c r="H15" s="44" t="str" cm="1">
         <f t="array" ref="H15">_xlfn.IFS($H$4="On Demand", "Requests (Hour)", $H$4="Provisioned Capacity", "Capacity Units (Hour)")</f>
-        <v>Capacity Units (Hour)</v>
+        <v>Requests (Hour)</v>
       </c>
       <c r="I15" s="44" t="str" cm="1">
         <f t="array" ref="I15">_xlfn.IFS($H$4="On Demand", "Requests (Month)", $H$4="Provisioned Capacity", "Capacity Units (Month)")</f>
-        <v>Capacity Units (Month)</v>
+        <v>Requests (Month)</v>
       </c>
       <c r="J15" s="44" t="s">
         <v>119</v>
@@ -7274,113 +7224,113 @@
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="147"/>
-      <c r="D16" s="138" t="s">
+      <c r="C16" s="134"/>
+      <c r="D16" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="139"/>
+      <c r="E16" s="142"/>
       <c r="G16" s="46" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.IFS($H$4="On Demand", "RRU", $H$4="Provisioned Capacity", "RCU")</f>
-        <v>RCU</v>
+        <v>RRU</v>
       </c>
       <c r="H16" s="62" cm="1">
         <f t="array" ref="H16">_xlfn.IFS($H$4="Provisioned Capacity",(CEILING($H$6,4)/4)*(($H$11*(H8/100))*0.5+($H$11*(($H$9/100)))+($H$11*($H$10/100))*2)*(1/I4),$H$4="On Demand",(CEILING($H$6,4)/4)*(($H$11*($H$8/100))*0.5+($H$11*(($H$9/100)))+($H$11*(($H$10/100))*2))*3600*(I4))</f>
-        <v>71.428571428571431</v>
+        <v>1080000</v>
       </c>
       <c r="I16" s="62">
         <f>$H$16*730</f>
-        <v>52142.857142857145</v>
+        <v>788400000</v>
       </c>
       <c r="J16" s="68" cm="1">
         <f t="array" ref="J16">_xlfn.IFS($H$4="Provisioned Capacity",$I$16*$H$30,$H$4="On Demand",$I$16*$L$30/1000000)</f>
-        <v>7.665</v>
-      </c>
-      <c r="K16" s="136">
+        <v>98.55</v>
+      </c>
+      <c r="K16" s="166">
         <f>$J$16+$J$17</f>
-        <v>160.965</v>
-      </c>
-      <c r="L16" s="130">
+        <v>98.55</v>
+      </c>
+      <c r="L16" s="160">
         <f>$K$16+$K$18</f>
-        <v>160.965</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="148">
+      <c r="B17" s="135">
         <v>1251</v>
       </c>
-      <c r="C17" s="149"/>
-      <c r="D17" s="140" cm="1">
+      <c r="C17" s="136"/>
+      <c r="D17" s="143" cm="1">
         <f t="array" ref="D17">_xlfn.IFS(H4="Provisioned capacity",B17/I36,H4="On Demand",B17/M36)</f>
-        <v>999.98368678629686</v>
-      </c>
-      <c r="E17" s="141"/>
+        <v>1008.8709677419355</v>
+      </c>
+      <c r="E17" s="144"/>
       <c r="G17" s="47" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.IFS($H$4="On Demand", "WRU", $H$4="Provisioned Capacity", "WCU")</f>
-        <v>WCU</v>
+        <v>WRU</v>
       </c>
       <c r="H17" s="64" cm="1">
         <f t="array" ref="H17">_xlfn.IFS($H$4="Provisioned Capacity",(CEILING($H$6,1)/1)*(($H$12*($I$10/100))*2+($H$12*(1-($I$10/100))))*(1/I4),$H$4="On Demand",(CEILING($H$6,1)/1)*(($H$12*($I$10/100))*3600*2+($H$12*(1-($I$10/100))*3600))*I4)</f>
-        <v>285.71428571428572</v>
+        <v>0</v>
       </c>
       <c r="I17" s="64">
         <f>H17*730</f>
-        <v>208571.42857142858</v>
+        <v>0</v>
       </c>
       <c r="J17" s="69" cm="1">
         <f t="array" ref="J17">_xlfn.IFS($H$4="Provisioned Capacity",$I$17*$G$30,$H$4="On Demand",$I$17*$K$30/1000000)</f>
-        <v>153.30000000000001</v>
-      </c>
-      <c r="K17" s="137"/>
-      <c r="L17" s="131"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="167"/>
+      <c r="L17" s="161"/>
     </row>
     <row r="18" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="150">
+      <c r="B18" s="148">
         <v>200</v>
       </c>
-      <c r="C18" s="151"/>
-      <c r="D18" s="142">
+      <c r="C18" s="149"/>
+      <c r="D18" s="145">
         <f>B18/P36</f>
         <v>500</v>
       </c>
-      <c r="E18" s="143"/>
+      <c r="E18" s="130"/>
       <c r="G18" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="125">
+      <c r="H18" s="155">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="126"/>
-      <c r="J18" s="127"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="157"/>
       <c r="K18" s="45">
         <f>IF($H$13&gt;25,$H$13*$O$30-25*$O$30,0)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="132"/>
+      <c r="L18" s="162"/>
     </row>
     <row r="19" spans="1:16" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="152">
+      <c r="B19" s="150">
         <f>SUM(B17:B18)</f>
         <v>1451</v>
       </c>
-      <c r="C19" s="153"/>
-      <c r="D19" s="144">
+      <c r="C19" s="151"/>
+      <c r="D19" s="146">
         <f>SUM(D17:D18)</f>
-        <v>1499.9836867862969</v>
-      </c>
-      <c r="E19" s="145"/>
+        <v>1508.8709677419356</v>
+      </c>
+      <c r="E19" s="147"/>
       <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7404,11 +7354,11 @@
       </c>
       <c r="H20" s="44" t="str" cm="1">
         <f t="array" ref="H20">_xlfn.IFS($H$4="On Demand", "Requests (Hour)", $H$4="Provisioned Capacity", "Capacity Units (Hour)")</f>
-        <v>Capacity Units (Hour)</v>
+        <v>Requests (Hour)</v>
       </c>
       <c r="I20" s="44" t="str" cm="1">
         <f t="array" ref="I20">_xlfn.IFS($H$4="On Demand", "Requests (Month)", $H$4="Provisioned Capacity", "Capacity Units (Month)")</f>
-        <v>Capacity Units (Month)</v>
+        <v>Requests (Month)</v>
       </c>
       <c r="J20" s="44" t="s">
         <v>119</v>
@@ -7439,31 +7389,31 @@
       </c>
       <c r="E21" s="17" cm="1">
         <f t="array" ref="E21">_xlfn.IFS(H4="Provisioned capacity",(1-1/I36)*B17-(1/P36-1)*B18,H4="On Demand",(1-1/M36)*B17-(1/P36-1)*B18)</f>
-        <v>-48.983686786296744</v>
+        <v>-57.870967741935573</v>
       </c>
       <c r="G21" s="49" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.IFS($H$4="On Demand", "RRU", $H$4="Provisioned Capacity", "RCU")</f>
-        <v>RCU</v>
+        <v>RRU</v>
       </c>
       <c r="H21" s="66" cm="1">
         <f t="array" ref="H21">_xlfn.IFS($H$4="Provisioned Capacity",(CEILING($H$6,4)/4)*(($H$11*(H8/100))*0.5+($H$11*(($H$9/100)))+($H$11*($H$10/100))*2)*(1/I4),$H$4="On Demand",(CEILING($H$6,4)/4)*(($H$11*($H$8/100))*0.5+($H$11*(($H$9/100)))+($H$11*(($H$10/100)))*2)*3600)</f>
-        <v>71.428571428571431</v>
+        <v>1080000</v>
       </c>
       <c r="I21" s="62">
         <f>$H$21*730</f>
-        <v>52142.857142857145</v>
+        <v>788400000</v>
       </c>
       <c r="J21" s="63" cm="1">
         <f t="array" ref="J21">_xlfn.IFS($H$4="Provisioned Capacity",$I$21*$J$30,$H$4="On Demand",$I$21*$N$30/1000000)</f>
-        <v>9.5942857142857143</v>
-      </c>
-      <c r="K21" s="136">
+        <v>122.202</v>
+      </c>
+      <c r="K21" s="166">
         <f>$J$21+$J$22</f>
-        <v>201.27142857142857</v>
-      </c>
-      <c r="L21" s="133">
+        <v>122.202</v>
+      </c>
+      <c r="L21" s="163">
         <f>$K$21+$K$23</f>
-        <v>201.27142857142857</v>
+        <v>122.202</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7475,38 +7425,38 @@
       </c>
       <c r="G22" s="49" t="str" cm="1">
         <f t="array" ref="G22">_xlfn.IFS($H$4="On Demand", "WRU", $H$4="Provisioned Capacity", "WCU")</f>
-        <v>WCU</v>
+        <v>WRU</v>
       </c>
       <c r="H22" s="67" cm="1">
         <f t="array" ref="H22">_xlfn.IFS($H$4="Provisioned Capacity",(CEILING($H$6,1)/1)*(($H$12*($I$10/100))*2+($H$12*(1-($I$10/100))))*(1/I4),$H$4="On Demand",(CEILING($H$6,1)/1)*(($H$12*($I$10/100))*3600*2+($H$12*(1-($I$10/100))*3600)))</f>
-        <v>285.71428571428572</v>
+        <v>0</v>
       </c>
       <c r="I22" s="64">
         <f>H22*730</f>
-        <v>208571.42857142858</v>
+        <v>0</v>
       </c>
       <c r="J22" s="65" cm="1">
         <f t="array" ref="J22">_xlfn.IFS($H$4="Provisioned Capacity",$I$22*$I$30,$H$4="On Demand",$I$22*$M$30/1000000)</f>
-        <v>191.67714285714285</v>
-      </c>
-      <c r="K22" s="137"/>
-      <c r="L22" s="134"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="167"/>
+      <c r="L22" s="164"/>
     </row>
     <row r="23" spans="1:16" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="H23" s="128">
+      <c r="H23" s="158">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="126"/>
-      <c r="J23" s="127"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="45">
         <f>IF($H$13&gt;25,$H$13*$P$30-25*$P$30,0)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="135"/>
+      <c r="L23" s="165"/>
     </row>
     <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -7528,7 +7478,7 @@
       </c>
       <c r="H26" s="54" cm="1">
         <f t="array" ref="H26">_xlfn.IFS($G$26="Candidate to Standard",$L$21-$L$16,$G$26="Candidate to Standard-IA",$L$16-$L$21,$G$26="Even", 0)</f>
-        <v>40.306428571428569</v>
+        <v>23.652000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7574,43 +7524,43 @@
     <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G30" s="32">
         <f>VLOOKUP($H$5,Table4[#All],7,0)</f>
-        <v>7.3499999999999998E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],8,0)</f>
-        <v>1.47E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],9,0)</f>
-        <v>9.19E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],10,0)</f>
-        <v>1.84E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],11,0)</f>
-        <v>1.4135</v>
+        <v>0.625</v>
       </c>
       <c r="L30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],12,0)</f>
-        <v>0.28299999999999997</v>
+        <v>0.125</v>
       </c>
       <c r="M30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],13,0)</f>
-        <v>1.7668999999999999</v>
+        <v>0.78</v>
       </c>
       <c r="N30" s="33">
         <f>VLOOKUP($H$5,Table4[#All],14,0)</f>
-        <v>0.35399999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="O30" s="30">
         <f>VLOOKUP($H$5,Table4[#All],5,0)</f>
-        <v>0.28299999999999997</v>
+        <v>0.25</v>
       </c>
       <c r="P30" s="31">
         <f>VLOOKUP($H$5,Table4[#All],6,0)</f>
-        <v>0.1132</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33" spans="8:16" hidden="1" x14ac:dyDescent="0.2"/>
@@ -7618,38 +7568,38 @@
     <row r="35" spans="8:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="I35">
         <f>$I$30/$G$30</f>
-        <v>1.2503401360544217</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="J35">
         <f>$J$30/$H$30</f>
-        <v>1.2517006802721089</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="M35">
         <f>$M$30/$K$30</f>
-        <v>1.2500176865935619</v>
+        <v>1.248</v>
       </c>
       <c r="N35">
         <f>$N$30/$L$30</f>
-        <v>1.2508833922261484</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="36" spans="8:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="H36" t="s">
         <v>132</v>
       </c>
-      <c r="I36" s="129">
+      <c r="I36" s="159">
         <f>$J$35*($H$11/($H$11+$H$12))+$I$35*($H$12/($H$12+$H$11))</f>
-        <v>1.2510204081632654</v>
-      </c>
-      <c r="J36" s="129"/>
+        <v>1.2307692307692311</v>
+      </c>
+      <c r="J36" s="159"/>
       <c r="L36" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="129">
+      <c r="M36" s="159">
         <f>$N$35*($H$11/($H$11+$H$12))+$M$35*($H$12/($H$12+$H$11))</f>
-        <v>1.2504505394098553</v>
-      </c>
-      <c r="N36" s="129"/>
+        <v>1.24</v>
+      </c>
+      <c r="N36" s="159"/>
       <c r="P36">
         <f>$P$30/$O$30</f>
         <v>0.4</v>
@@ -7660,6 +7610,23 @@
     <row r="40" spans="8:16" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -7670,23 +7637,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K16:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="lessThan">
@@ -7786,8 +7736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF287C15-877C-2B4D-AD91-43E51C53AD46}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7796,7 +7746,7 @@
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="32.1640625" customWidth="1"/>
     <col min="4" max="4" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -7814,67 +7764,68 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="156"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
     </row>
     <row r="4" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="186"/>
-      <c r="D4" s="157" t="s">
+      <c r="C4" s="172"/>
+      <c r="D4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="183">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="185">
+      <c r="B5" s="168">
+        <f>586+821</f>
+        <v>1407</v>
+      </c>
+      <c r="C5" s="169"/>
+      <c r="D5" s="170">
         <f>B5*1.25</f>
-        <v>1250</v>
-      </c>
-      <c r="E5" s="160"/>
+        <v>1758.75</v>
+      </c>
+      <c r="E5" s="128"/>
     </row>
     <row r="6" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="174">
-        <v>100</v>
-      </c>
-      <c r="C6" s="175"/>
-      <c r="D6" s="176">
+      <c r="B6" s="179">
+        <v>2584</v>
+      </c>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181">
         <f>B6*0.4</f>
-        <v>40</v>
-      </c>
-      <c r="E6" s="177"/>
+        <v>1033.6000000000001</v>
+      </c>
+      <c r="E6" s="182"/>
     </row>
     <row r="7" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="171">
+      <c r="B7" s="176">
         <f>SUM(B5:B6)</f>
-        <v>1100</v>
-      </c>
-      <c r="C7" s="172"/>
-      <c r="D7" s="178">
+        <v>3991</v>
+      </c>
+      <c r="C7" s="177"/>
+      <c r="D7" s="183">
         <f>SUM(D5:D6)</f>
-        <v>1290</v>
-      </c>
-      <c r="E7" s="179"/>
+        <v>2792.3500000000004</v>
+      </c>
+      <c r="E7" s="184"/>
     </row>
     <row r="8" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -7897,23 +7848,23 @@
     <row r="9" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <f>B6/B5</f>
-        <v>0.1</v>
+        <v>1.8365316275764036</v>
       </c>
       <c r="B9" s="9">
         <f>B5*0.416667</f>
-        <v>416.66700000000003</v>
+        <v>586.25046900000007</v>
       </c>
       <c r="C9" s="10">
         <f>B6</f>
-        <v>100</v>
+        <v>2584</v>
       </c>
       <c r="D9" s="16" t="str">
         <f>IF(C9&gt;B9, "Candidate to Standard-IA","Optimized")</f>
-        <v>Optimized</v>
+        <v>Candidate to Standard-IA</v>
       </c>
       <c r="E9" s="17">
         <f>0.6*B6 - 0.25*B5</f>
-        <v>-190</v>
+        <v>1198.6499999999999</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -7957,67 +7908,67 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="155"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="156"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
     </row>
     <row r="16" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="180" t="s">
+      <c r="C16" s="141"/>
+      <c r="D16" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="139"/>
+      <c r="E16" s="142"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="181">
+      <c r="B17" s="185">
         <v>6000</v>
       </c>
-      <c r="C17" s="182"/>
-      <c r="D17" s="159">
+      <c r="C17" s="186"/>
+      <c r="D17" s="127">
         <f>B17/1.25</f>
         <v>4800</v>
       </c>
-      <c r="E17" s="160"/>
+      <c r="E17" s="128"/>
     </row>
     <row r="18" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="168">
+      <c r="B18" s="173">
         <v>168</v>
       </c>
-      <c r="C18" s="169"/>
-      <c r="D18" s="170">
+      <c r="C18" s="174"/>
+      <c r="D18" s="175">
         <f>B18/0.4</f>
         <v>420</v>
       </c>
-      <c r="E18" s="143"/>
+      <c r="E18" s="130"/>
     </row>
     <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="171">
+      <c r="B19" s="176">
         <f>SUM(B17:B18)</f>
         <v>6168</v>
       </c>
-      <c r="C19" s="172"/>
-      <c r="D19" s="173">
+      <c r="C19" s="177"/>
+      <c r="D19" s="178">
         <f>SUM(D17:D18)</f>
         <v>5220</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="147"/>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
@@ -8073,11 +8024,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B19:C19"/>
@@ -8091,6 +8037,11 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="A9">
     <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="lessThan">
@@ -8155,8 +8106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE3DC98-ECA8-E340-8618-C286BC8288EE}">
   <dimension ref="A2:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8242,178 +8193,178 @@
     </row>
     <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="E3" s="27">
-        <v>0.25</v>
+        <v>0.33677000000000001</v>
       </c>
       <c r="F3" s="27">
-        <v>0.1</v>
+        <v>0.13471</v>
       </c>
       <c r="G3" s="26">
-        <v>6.4999999999999997E-4</v>
+        <v>8.7465000000000004E-4</v>
       </c>
       <c r="H3" s="26">
-        <v>1.2999999999999999E-4</v>
+        <v>1.7493000000000001E-4</v>
       </c>
       <c r="I3" s="26">
-        <v>8.0999999999999996E-4</v>
+        <v>9.6469999999999998E-4</v>
       </c>
       <c r="J3" s="26">
-        <v>1.6000000000000001E-4</v>
+        <v>2.187E-4</v>
       </c>
       <c r="K3" s="28">
-        <v>1.25</v>
+        <v>0.84</v>
       </c>
       <c r="L3" s="28">
-        <v>0.25</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="M3" s="28">
-        <v>1.56</v>
+        <v>1.05</v>
       </c>
       <c r="N3" s="28">
-        <v>0.31</v>
+        <v>0.21049999999999999</v>
       </c>
       <c r="O3" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2461538461538462</v>
+        <v>1.1029554679014462</v>
       </c>
       <c r="P3" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2307692307692311</v>
+        <v>1.2502143714628708</v>
       </c>
       <c r="Q3" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.248</v>
+        <v>1.25</v>
       </c>
       <c r="R3" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.24</v>
+        <v>1.2529761904761905</v>
       </c>
       <c r="S3" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.40000593877126822</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="E4" s="27">
-        <v>0.28000000000000003</v>
+        <v>0.3135</v>
       </c>
       <c r="F4" s="27">
-        <v>0.112</v>
+        <v>0.12540000000000001</v>
       </c>
       <c r="G4" s="26">
-        <v>7.2499999999999995E-4</v>
+        <v>8.1400000000000005E-4</v>
       </c>
       <c r="H4" s="26">
-        <v>1.45E-4</v>
+        <v>1.628E-4</v>
       </c>
       <c r="I4" s="26">
-        <v>9.0600000000000001E-4</v>
+        <v>1.018E-3</v>
       </c>
       <c r="J4" s="26">
-        <v>1.8100000000000001E-4</v>
+        <v>2.0350000000000001E-4</v>
       </c>
       <c r="K4" s="28">
-        <v>1.3942000000000001</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="L4" s="28">
-        <v>0.27900000000000003</v>
+        <v>0.155</v>
       </c>
       <c r="M4" s="28">
-        <v>1.7427999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="N4" s="28">
-        <v>0.34899999999999998</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="O4" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2496551724137932</v>
+        <v>1.2506142506142506</v>
       </c>
       <c r="P4" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2482758620689656</v>
+        <v>1.25</v>
       </c>
       <c r="Q4" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500358628604216</v>
+        <v>1.2484076433121019</v>
       </c>
       <c r="R4" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25089605734767</v>
+        <v>1.2580645161290323</v>
       </c>
       <c r="S4" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E5" s="27">
-        <v>0.3</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F5" s="27">
-        <v>0.12</v>
+        <v>0.114</v>
       </c>
       <c r="G5" s="26">
-        <v>7.7999999999999999E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H5" s="26">
-        <v>1.56E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I5" s="26">
-        <v>9.7499999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J5" s="26">
-        <v>1.95E-4</v>
+        <v>1.85E-4</v>
       </c>
       <c r="K5" s="28">
-        <v>1.5</v>
+        <v>0.71</v>
       </c>
       <c r="L5" s="28">
-        <v>0.3</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M5" s="28">
-        <v>1.875</v>
+        <v>0.89</v>
       </c>
       <c r="N5" s="28">
-        <v>0.375</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O5" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P5" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
@@ -8421,11 +8372,11 @@
       </c>
       <c r="Q5" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R5" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S5" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8434,62 +8385,62 @@
     </row>
     <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E6" s="27">
-        <v>0.3</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F6" s="27">
-        <v>0.12</v>
+        <v>0.114</v>
       </c>
       <c r="G6" s="26">
-        <v>7.7999999999999999E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H6" s="26">
-        <v>1.56E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I6" s="26">
-        <v>9.7499999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J6" s="26">
-        <v>1.95E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K6" s="28">
-        <v>1.5</v>
+        <v>0.71</v>
       </c>
       <c r="L6" s="28">
-        <v>0.3</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M6" s="28">
-        <v>1.875</v>
+        <v>0.89</v>
       </c>
       <c r="N6" s="28">
-        <v>0.375</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O6" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P6" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q6" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R6" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S6" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8498,62 +8449,62 @@
     </row>
     <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="E7" s="27">
-        <v>0.25</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F7" s="27">
-        <v>0.1</v>
+        <v>0.114</v>
       </c>
       <c r="G7" s="26">
-        <v>6.4999999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H7" s="26">
-        <v>1.2999999999999999E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I7" s="26">
-        <v>8.0999999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J7" s="26">
-        <v>1.6000000000000001E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K7" s="28">
-        <v>1.25</v>
+        <v>0.71</v>
       </c>
       <c r="L7" s="28">
-        <v>0.25</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M7" s="28">
-        <v>1.56</v>
+        <v>0.89</v>
       </c>
       <c r="N7" s="28">
-        <v>0.31</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O7" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2461538461538462</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P7" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2307692307692311</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q7" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.248</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R7" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.24</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S7" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8562,62 +8513,62 @@
     </row>
     <row r="8" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E8" s="27">
-        <v>0.25</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F8" s="27">
-        <v>0.1</v>
+        <v>0.114</v>
       </c>
       <c r="G8" s="26">
-        <v>6.4999999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H8" s="26">
-        <v>1.2999999999999999E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I8" s="26">
-        <v>8.0999999999999996E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J8" s="26">
-        <v>1.6000000000000001E-4</v>
+        <v>1.85E-4</v>
       </c>
       <c r="K8" s="28">
-        <v>1.25</v>
+        <v>0.71</v>
       </c>
       <c r="L8" s="28">
-        <v>0.25</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M8" s="28">
-        <v>1.56</v>
+        <v>0.89</v>
       </c>
       <c r="N8" s="28">
-        <v>0.31</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O8" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2461538461538462</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P8" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2307692307692311</v>
+        <v>1.25</v>
       </c>
       <c r="Q8" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.248</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R8" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.24</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S8" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -8626,302 +8577,302 @@
     </row>
     <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="E9" s="27">
-        <v>0.375</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F9" s="27">
-        <v>0.15</v>
+        <v>0.114</v>
       </c>
       <c r="G9" s="26">
-        <v>9.7499999999999996E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="H9" s="26">
-        <v>1.95E-4</v>
+        <v>1.484E-4</v>
       </c>
       <c r="I9" s="26">
-        <v>1.219E-3</v>
+        <v>9.2800000000000001E-4</v>
       </c>
       <c r="J9" s="26">
-        <v>2.4399999999999999E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K9" s="28">
-        <v>1.875</v>
+        <v>0.71</v>
       </c>
       <c r="L9" s="28">
-        <v>0.375</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M9" s="28">
-        <v>2.3439999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="N9" s="28">
-        <v>0.46899999999999997</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O9" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2502564102564104</v>
+        <v>1.2506738544474394</v>
       </c>
       <c r="P9" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2512820512820513</v>
+        <v>1.25</v>
       </c>
       <c r="Q9" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2501333333333333</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R9" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2506666666666666</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S9" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E10" s="27">
-        <v>0.31130000000000002</v>
+        <v>0.27074999999999999</v>
       </c>
       <c r="F10" s="27">
-        <v>0.1245</v>
+        <v>0.10829999999999999</v>
       </c>
       <c r="G10" s="26">
-        <v>8.0849999999999997E-4</v>
+        <v>7.0489999999999995E-4</v>
       </c>
       <c r="H10" s="26">
-        <v>1.617E-4</v>
+        <v>1.4098E-4</v>
       </c>
       <c r="I10" s="26">
-        <v>1.0106E-3</v>
+        <v>8.811E-4</v>
       </c>
       <c r="J10" s="26">
-        <v>2.0210000000000001E-4</v>
+        <v>1.762E-4</v>
       </c>
       <c r="K10" s="28">
-        <v>1.5548999999999999</v>
-      </c>
-      <c r="L10" s="28">
-        <v>0.311</v>
+        <v>0.68</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0.13550000000000001</v>
       </c>
       <c r="M10" s="28">
-        <v>1.9436</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="N10" s="28">
-        <v>0.38900000000000001</v>
+        <v>0.16950000000000001</v>
       </c>
       <c r="O10" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2499690785405071</v>
+        <v>1.2499645339764507</v>
       </c>
       <c r="P10" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2498453927025357</v>
+        <v>1.2498226698822528</v>
       </c>
       <c r="Q10" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499839217956139</v>
+        <v>1.2426470588235292</v>
       </c>
       <c r="R10" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508038585209003</v>
+        <v>1.2509225092250922</v>
       </c>
       <c r="S10" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39993575329264375</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="E11" s="27">
-        <v>0.31130000000000002</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F11" s="27">
-        <v>0.12452000000000001</v>
+        <v>0.114</v>
       </c>
       <c r="G11" s="26">
-        <v>8.0849999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H11" s="26">
-        <v>1.617E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I11" s="26">
-        <v>1.0108999999999999E-3</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J11" s="26">
-        <v>2.0239999999999999E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K11" s="28">
-        <v>1.5509999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="L11" s="28">
-        <v>0.31130000000000002</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M11" s="28">
-        <v>1.9470000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="N11" s="28">
-        <v>0.38940000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O11" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P11" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721087</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q11" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2553191489361704</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R11" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508833922261484</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S11" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E12" s="27">
-        <v>0.33960000000000001</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F12" s="27">
-        <v>0.13583999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="G12" s="26">
-        <v>8.8199999999999997E-4</v>
+        <v>7.3999999999999999E-4</v>
       </c>
       <c r="H12" s="26">
-        <v>1.7640000000000001E-4</v>
+        <v>1.4799999999999999E-4</v>
       </c>
       <c r="I12" s="26">
-        <v>1.1027999999999999E-3</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="J12" s="26">
-        <v>2.208E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K12" s="28">
-        <v>1.6961999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="L12" s="28">
-        <v>0.33960000000000001</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M12" s="28">
-        <v>2.1202999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="N12" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O12" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.2567567567567568</v>
       </c>
       <c r="P12" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721089</v>
+        <v>1.2533783783783785</v>
       </c>
       <c r="Q12" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500294776559369</v>
+        <v>1.2535211267605635</v>
       </c>
       <c r="R12" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.0424028268551235</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S12" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E13" s="27">
-        <v>0.29715000000000003</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F13" s="27">
-        <v>0.11885999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="G13" s="26">
-        <v>7.7200000000000001E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="H13" s="26">
-        <v>1.5440000000000001E-4</v>
+        <v>1.484E-4</v>
       </c>
       <c r="I13" s="26">
-        <v>9.6500000000000004E-4</v>
+        <v>9.2750000000000005E-4</v>
       </c>
       <c r="J13" s="26">
-        <v>1.93E-4</v>
+        <v>1.8550000000000001E-4</v>
       </c>
       <c r="K13" s="28">
-        <v>1.4845999999999999</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="L13" s="28">
-        <v>0.29699999999999999</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="M13" s="28">
-        <v>1.8557999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="N13" s="28">
-        <v>0.371</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="O13" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
@@ -8933,59 +8884,59 @@
       </c>
       <c r="Q13" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500336791054829</v>
+        <v>1.2447552447552448</v>
       </c>
       <c r="R13" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2491582491582491</v>
+        <v>1.249122807017544</v>
       </c>
       <c r="S13" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E14" s="27">
-        <v>0.29715000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="F14" s="27">
-        <v>0.11885999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="G14" s="26">
-        <v>7.7200000000000001E-4</v>
+        <v>7.7999999999999999E-4</v>
       </c>
       <c r="H14" s="26">
-        <v>1.5440000000000001E-4</v>
+        <v>1.56E-4</v>
       </c>
       <c r="I14" s="26">
-        <v>9.6500000000000004E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="J14" s="26">
-        <v>1.93E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="K14" s="28">
-        <v>1.4845999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="L14" s="28">
-        <v>0.29699999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="M14" s="28">
-        <v>1.8557999999999999</v>
+        <v>0.9375</v>
       </c>
       <c r="N14" s="28">
-        <v>0.371</v>
+        <v>0.1875</v>
       </c>
       <c r="O14" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
@@ -8997,75 +8948,75 @@
       </c>
       <c r="Q14" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500336791054829</v>
+        <v>1.25</v>
       </c>
       <c r="R14" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2491582491582491</v>
+        <v>1.25</v>
       </c>
       <c r="S14" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E15" s="27">
-        <v>0.28299999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="F15" s="27">
-        <v>0.1132</v>
+        <v>0.12</v>
       </c>
       <c r="G15" s="26">
-        <v>7.3499999999999998E-4</v>
+        <v>7.7999999999999999E-4</v>
       </c>
       <c r="H15" s="26">
-        <v>1.47E-4</v>
+        <v>1.56E-4</v>
       </c>
       <c r="I15" s="26">
-        <v>9.19E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="J15" s="26">
-        <v>1.84E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="K15" s="28">
-        <v>1.4135</v>
+        <v>0.75</v>
       </c>
       <c r="L15" s="28">
-        <v>0.28299999999999997</v>
+        <v>0.15</v>
       </c>
       <c r="M15" s="28">
-        <v>1.7668999999999999</v>
+        <v>0.9375</v>
       </c>
       <c r="N15" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.1875</v>
       </c>
       <c r="O15" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.25</v>
       </c>
       <c r="P15" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721089</v>
+        <v>1.25</v>
       </c>
       <c r="Q15" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500176865935619</v>
+        <v>1.25</v>
       </c>
       <c r="R15" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508833922261484</v>
+        <v>1.25</v>
       </c>
       <c r="S15" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9074,126 +9025,126 @@
     </row>
     <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E16" s="27">
-        <v>0.28299999999999997</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F16" s="27">
-        <v>0.1132</v>
+        <v>0.11</v>
       </c>
       <c r="G16" s="26">
-        <v>7.3499999999999998E-4</v>
+        <v>7.1500000000000003E-4</v>
       </c>
       <c r="H16" s="26">
-        <v>1.47E-4</v>
+        <v>1.4300000000000001E-4</v>
       </c>
       <c r="I16" s="26">
-        <v>9.19E-4</v>
+        <v>8.9400000000000005E-4</v>
       </c>
       <c r="J16" s="26">
-        <v>1.84E-4</v>
+        <v>1.7899999999999999E-4</v>
       </c>
       <c r="K16" s="28">
-        <v>1.4135</v>
+        <v>0.6875</v>
       </c>
       <c r="L16" s="28">
-        <v>0.28299999999999997</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M16" s="28">
-        <v>1.7668999999999999</v>
+        <v>0.85950000000000004</v>
       </c>
       <c r="N16" s="28">
-        <v>0.35399999999999998</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="O16" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503401360544217</v>
+        <v>1.2503496503496503</v>
       </c>
       <c r="P16" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517006802721089</v>
+        <v>1.2517482517482517</v>
       </c>
       <c r="Q16" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500176865935619</v>
+        <v>1.2501818181818183</v>
       </c>
       <c r="R16" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508833922261484</v>
+        <v>1.2509090909090907</v>
       </c>
       <c r="S16" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="E17" s="27">
-        <v>0.29715000000000003</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F17" s="27">
-        <v>0.11885999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="G17" s="26">
-        <v>7.7174999999999998E-4</v>
+        <v>7.1500000000000003E-4</v>
       </c>
       <c r="H17" s="26">
-        <v>1.5435000000000001E-4</v>
+        <v>1.4300000000000001E-4</v>
       </c>
       <c r="I17" s="26">
-        <v>9.6469999999999998E-4</v>
+        <v>8.9400000000000005E-4</v>
       </c>
       <c r="J17" s="26">
-        <v>1.93E-4</v>
+        <v>1.7899999999999999E-4</v>
       </c>
       <c r="K17" s="28">
-        <v>1.4842</v>
+        <v>0.6875</v>
       </c>
       <c r="L17" s="28">
-        <v>0.29680000000000001</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M17" s="28">
-        <v>1.8552999999999999</v>
+        <v>0.85950000000000004</v>
       </c>
       <c r="N17" s="28">
-        <v>0.371</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="O17" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2500161969549726</v>
+        <v>1.2503496503496503</v>
       </c>
       <c r="P17" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2504049238743116</v>
+        <v>1.2517482517482517</v>
       </c>
       <c r="Q17" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500336881821856</v>
+        <v>1.2501818181818183</v>
       </c>
       <c r="R17" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.25</v>
+        <v>1.2509090909090907</v>
       </c>
       <c r="S17" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9202,62 +9153,62 @@
     </row>
     <row r="18" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E18" s="27">
-        <v>0.26900000000000002</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="F18" s="27">
-        <v>0.1076</v>
+        <v>0.12239999999999999</v>
       </c>
       <c r="G18" s="26">
-        <v>6.9800000000000005E-4</v>
+        <v>7.9299999999999998E-4</v>
       </c>
       <c r="H18" s="26">
-        <v>1.3999999999999999E-4</v>
+        <v>1.5860000000000001E-4</v>
       </c>
       <c r="I18" s="26">
-        <v>8.7250000000000001E-4</v>
+        <v>9.9099999999999991E-4</v>
       </c>
       <c r="J18" s="26">
-        <v>1.75E-4</v>
+        <v>1.983E-4</v>
       </c>
       <c r="K18" s="28">
-        <v>1.3428</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="L18" s="28">
-        <v>0.26900000000000002</v>
+        <v>0.1525</v>
       </c>
       <c r="M18" s="28">
-        <v>1.6785000000000001</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="N18" s="28">
-        <v>0.33600000000000002</v>
+        <v>0.1905</v>
       </c>
       <c r="O18" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2496847414880201</v>
       </c>
       <c r="P18" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2503152585119797</v>
       </c>
       <c r="Q18" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.2524590163934426</v>
       </c>
       <c r="R18" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2490706319702602</v>
+        <v>1.2491803278688525</v>
       </c>
       <c r="S18" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9266,62 +9217,62 @@
     </row>
     <row r="19" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="E19" s="27">
-        <v>0.33660000000000001</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="F19" s="27">
-        <v>0.13464000000000001</v>
+        <v>0.1132</v>
       </c>
       <c r="G19" s="26">
-        <v>8.7200000000000005E-4</v>
+        <v>7.3499999999999998E-4</v>
       </c>
       <c r="H19" s="26">
-        <v>1.75E-4</v>
+        <v>1.47E-4</v>
       </c>
       <c r="I19" s="26">
-        <v>1.0901000000000001E-3</v>
+        <v>9.19E-4</v>
       </c>
       <c r="J19" s="26">
-        <v>2.1800000000000001E-4</v>
+        <v>1.84E-4</v>
       </c>
       <c r="K19" s="28">
-        <v>1.67</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="L19" s="28">
-        <v>0.33600000000000002</v>
+        <v>0.14149999999999999</v>
       </c>
       <c r="M19" s="28">
-        <v>2.101</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="N19" s="28">
-        <v>0.41899999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O19" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2501146788990827</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P19" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2457142857142858</v>
+        <v>1.2517006802721089</v>
       </c>
       <c r="Q19" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2580838323353294</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="R19" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2470238095238093</v>
+        <v>1.2508833922261484</v>
       </c>
       <c r="S19" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9330,62 +9281,62 @@
     </row>
     <row r="20" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E20" s="27">
-        <v>0.30599999999999999</v>
+        <v>0.29715000000000003</v>
       </c>
       <c r="F20" s="27">
-        <v>0.12239999999999999</v>
+        <v>0.11885999999999999</v>
       </c>
       <c r="G20" s="26">
-        <v>7.9299999999999998E-4</v>
+        <v>7.7200000000000001E-4</v>
       </c>
       <c r="H20" s="26">
-        <v>1.5860000000000001E-4</v>
+        <v>1.5440000000000001E-4</v>
       </c>
       <c r="I20" s="26">
-        <v>9.9099999999999991E-4</v>
+        <v>9.6500000000000004E-4</v>
       </c>
       <c r="J20" s="26">
-        <v>1.983E-4</v>
+        <v>1.93E-4</v>
       </c>
       <c r="K20" s="28">
-        <v>1.5249999999999999</v>
+        <v>0.74229999999999996</v>
       </c>
       <c r="L20" s="28">
-        <v>0.30499999999999999</v>
+        <v>0.1487</v>
       </c>
       <c r="M20" s="28">
-        <v>1.91</v>
+        <v>0.92789999999999995</v>
       </c>
       <c r="N20" s="28">
-        <v>0.38100000000000001</v>
+        <v>0.18559999999999999</v>
       </c>
       <c r="O20" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2496847414880201</v>
+        <v>1.25</v>
       </c>
       <c r="P20" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2503152585119797</v>
+        <v>1.25</v>
       </c>
       <c r="Q20" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2524590163934426</v>
+        <v>1.2500336791054829</v>
       </c>
       <c r="R20" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2491803278688525</v>
+        <v>1.2481506388702084</v>
       </c>
       <c r="S20" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9394,62 +9345,62 @@
     </row>
     <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E21" s="27">
-        <v>0.27500000000000002</v>
+        <v>0.29715000000000003</v>
       </c>
       <c r="F21" s="27">
-        <v>0.11</v>
+        <v>0.11885999999999999</v>
       </c>
       <c r="G21" s="26">
-        <v>7.1500000000000003E-4</v>
+        <v>7.7174999999999998E-4</v>
       </c>
       <c r="H21" s="26">
-        <v>1.4300000000000001E-4</v>
+        <v>1.5435000000000001E-4</v>
       </c>
       <c r="I21" s="26">
-        <v>8.9400000000000005E-4</v>
+        <v>9.6469999999999998E-4</v>
       </c>
       <c r="J21" s="26">
-        <v>1.7899999999999999E-4</v>
+        <v>1.93E-4</v>
       </c>
       <c r="K21" s="28">
-        <v>1.375</v>
+        <v>0.74</v>
       </c>
       <c r="L21" s="28">
-        <v>0.27500000000000002</v>
+        <v>0.1484</v>
       </c>
       <c r="M21" s="28">
-        <v>1.7190000000000001</v>
+        <v>0.92764999999999997</v>
       </c>
       <c r="N21" s="28">
-        <v>0.34399999999999997</v>
+        <v>0.1855</v>
       </c>
       <c r="O21" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503496503496503</v>
+        <v>1.2500161969549726</v>
       </c>
       <c r="P21" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517482517482517</v>
+        <v>1.2504049238743116</v>
       </c>
       <c r="Q21" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2501818181818183</v>
+        <v>1.253581081081081</v>
       </c>
       <c r="R21" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2509090909090907</v>
+        <v>1.25</v>
       </c>
       <c r="S21" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9458,62 +9409,62 @@
     </row>
     <row r="22" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E22" s="27">
-        <v>0.27500000000000002</v>
+        <v>0.29715000000000003</v>
       </c>
       <c r="F22" s="27">
-        <v>0.11</v>
+        <v>0.11885999999999999</v>
       </c>
       <c r="G22" s="26">
-        <v>7.1500000000000003E-4</v>
+        <v>7.7200000000000001E-4</v>
       </c>
       <c r="H22" s="26">
-        <v>1.4300000000000001E-4</v>
+        <v>1.5440000000000001E-4</v>
       </c>
       <c r="I22" s="26">
-        <v>8.9400000000000005E-4</v>
+        <v>9.6500000000000004E-4</v>
       </c>
       <c r="J22" s="26">
-        <v>1.7899999999999999E-4</v>
+        <v>1.93E-4</v>
       </c>
       <c r="K22" s="28">
-        <v>1.375</v>
+        <v>0.74229999999999996</v>
       </c>
       <c r="L22" s="28">
-        <v>0.27500000000000002</v>
+        <v>0.1487</v>
       </c>
       <c r="M22" s="28">
-        <v>1.7190000000000001</v>
+        <v>0.92789999999999995</v>
       </c>
       <c r="N22" s="28">
-        <v>0.34399999999999997</v>
+        <v>0.18559999999999999</v>
       </c>
       <c r="O22" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2503496503496503</v>
+        <v>1.25</v>
       </c>
       <c r="P22" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2517482517482517</v>
+        <v>1.25</v>
       </c>
       <c r="Q22" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2501818181818183</v>
+        <v>1.2500336791054829</v>
       </c>
       <c r="R22" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2509090909090907</v>
+        <v>1.2481506388702084</v>
       </c>
       <c r="S22" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9522,62 +9473,62 @@
     </row>
     <row r="23" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="F23" s="27">
-        <v>0.114</v>
+        <v>0.1132</v>
       </c>
       <c r="G23" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>7.3499999999999998E-4</v>
       </c>
       <c r="H23" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.47E-4</v>
       </c>
       <c r="I23" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>9.19E-4</v>
       </c>
       <c r="J23" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>1.84E-4</v>
       </c>
       <c r="K23" s="28">
-        <v>1.4231</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="L23" s="28">
-        <v>0.28460000000000002</v>
+        <v>0.14149999999999999</v>
       </c>
       <c r="M23" s="28">
-        <v>1.7788999999999999</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="N23" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O23" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P23" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.2517006802721089</v>
       </c>
       <c r="Q23" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="R23" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508784258608572</v>
+        <v>1.2508833922261484</v>
       </c>
       <c r="S23" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9586,126 +9537,126 @@
     </row>
     <row r="24" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E24" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="F24" s="27">
-        <v>0.114</v>
+        <v>0.1076</v>
       </c>
       <c r="G24" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>6.9800000000000005E-4</v>
       </c>
       <c r="H24" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="I24" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>8.7250000000000001E-4</v>
       </c>
       <c r="J24" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>1.75E-4</v>
       </c>
       <c r="K24" s="28">
-        <v>1.4231</v>
+        <v>0.67</v>
       </c>
       <c r="L24" s="28">
-        <v>0.28460000000000002</v>
+        <v>0.13450000000000001</v>
       </c>
       <c r="M24" s="28">
-        <v>1.7788999999999999</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="N24" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="O24" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.25</v>
       </c>
       <c r="P24" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.25</v>
       </c>
       <c r="Q24" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2447761194029849</v>
       </c>
       <c r="R24" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508784258608572</v>
+        <v>1.2490706319702602</v>
       </c>
       <c r="S24" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="E25" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.33660000000000001</v>
       </c>
       <c r="F25" s="27">
-        <v>0.114</v>
+        <v>0.13464000000000001</v>
       </c>
       <c r="G25" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.7200000000000005E-4</v>
       </c>
       <c r="H25" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.75E-4</v>
       </c>
       <c r="I25" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.0901000000000001E-3</v>
       </c>
       <c r="J25" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>2.1800000000000001E-4</v>
       </c>
       <c r="K25" s="28">
-        <v>1.4231</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="L25" s="28">
-        <v>0.28460000000000002</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="M25" s="28">
-        <v>1.7788999999999999</v>
+        <v>1.0505</v>
       </c>
       <c r="N25" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.20949999999999999</v>
       </c>
       <c r="O25" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2501146788990827</v>
       </c>
       <c r="P25" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.2457142857142858</v>
       </c>
       <c r="Q25" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2580838323353294</v>
       </c>
       <c r="R25" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2508784258608572</v>
+        <v>1.2470238095238093</v>
       </c>
       <c r="S25" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -9714,382 +9665,382 @@
     </row>
     <row r="26" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="E26" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.33960000000000001</v>
       </c>
       <c r="F26" s="27">
-        <v>0.114</v>
+        <v>0.13583999999999999</v>
       </c>
       <c r="G26" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.8199999999999997E-4</v>
       </c>
       <c r="H26" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.7640000000000001E-4</v>
       </c>
       <c r="I26" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.1027999999999999E-3</v>
       </c>
       <c r="J26" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>2.208E-4</v>
       </c>
       <c r="K26" s="28">
-        <v>1.4231</v>
+        <v>0.85</v>
       </c>
       <c r="L26" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.17</v>
       </c>
       <c r="M26" s="28">
-        <v>1.7788999999999999</v>
+        <v>1.06</v>
       </c>
       <c r="N26" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O26" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P26" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2533783783783785</v>
+        <v>1.2517006802721089</v>
       </c>
       <c r="Q26" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2470588235294118</v>
       </c>
       <c r="R26" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.0411764705882351</v>
       </c>
       <c r="S26" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E27" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.31130000000000002</v>
       </c>
       <c r="F27" s="27">
-        <v>0.114</v>
+        <v>0.1245</v>
       </c>
       <c r="G27" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.0849999999999997E-4</v>
       </c>
       <c r="H27" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.617E-4</v>
       </c>
       <c r="I27" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.0106E-3</v>
       </c>
       <c r="J27" s="26">
-        <v>1.85E-4</v>
+        <v>2.0210000000000001E-4</v>
       </c>
       <c r="K27" s="28">
-        <v>1.42</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="L27" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.1555</v>
       </c>
       <c r="M27" s="28">
-        <v>1.78</v>
+        <v>0.97</v>
       </c>
       <c r="N27" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.19450000000000001</v>
       </c>
       <c r="O27" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2499690785405071</v>
       </c>
       <c r="P27" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2498453927025357</v>
       </c>
       <c r="Q27" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2535211267605635</v>
+        <v>1.2516129032258063</v>
       </c>
       <c r="R27" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.2508038585209003</v>
       </c>
       <c r="S27" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39993575329264375</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="E28" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.31130000000000002</v>
       </c>
       <c r="F28" s="27">
-        <v>0.114</v>
+        <v>0.12452000000000001</v>
       </c>
       <c r="G28" s="26">
-        <v>7.3999999999999999E-4</v>
+        <v>8.0849999999999997E-4</v>
       </c>
       <c r="H28" s="26">
-        <v>1.4799999999999999E-4</v>
+        <v>1.617E-4</v>
       </c>
       <c r="I28" s="26">
-        <v>9.3000000000000005E-4</v>
+        <v>1.0108999999999999E-3</v>
       </c>
       <c r="J28" s="26">
-        <v>1.85E-4</v>
+        <v>2.0239999999999999E-4</v>
       </c>
       <c r="K28" s="28">
-        <v>1.4231</v>
+        <v>0.77549999999999997</v>
       </c>
       <c r="L28" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.15565000000000001</v>
       </c>
       <c r="M28" s="28">
-        <v>1.7788999999999999</v>
+        <v>0.97350000000000003</v>
       </c>
       <c r="N28" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.19450000000000001</v>
       </c>
       <c r="O28" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2567567567567568</v>
+        <v>1.2503401360544217</v>
       </c>
       <c r="P28" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2517006802721087</v>
       </c>
       <c r="Q28" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2500175672826925</v>
+        <v>1.2553191489361704</v>
       </c>
       <c r="R28" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.2495984580790234</v>
       </c>
       <c r="S28" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E29" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.375</v>
       </c>
       <c r="F29" s="27">
-        <v>0.114</v>
+        <v>0.15</v>
       </c>
       <c r="G29" s="26">
-        <v>7.4200000000000004E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="H29" s="26">
-        <v>1.484E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="I29" s="26">
-        <v>9.2800000000000001E-4</v>
+        <v>1.219E-3</v>
       </c>
       <c r="J29" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>2.4399999999999999E-4</v>
       </c>
       <c r="K29" s="28">
-        <v>1.4269000000000001</v>
+        <v>0.9375</v>
       </c>
       <c r="L29" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.1875</v>
       </c>
       <c r="M29" s="28">
-        <v>1.7836000000000001</v>
+        <v>1.1719999999999999</v>
       </c>
       <c r="N29" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.23449999999999999</v>
       </c>
       <c r="O29" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2506738544474394</v>
+        <v>1.2502564102564104</v>
       </c>
       <c r="P29" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2512820512820513</v>
       </c>
       <c r="Q29" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499824795010162</v>
+        <v>1.2501333333333333</v>
       </c>
       <c r="R29" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.2506666666666666</v>
       </c>
       <c r="S29" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E30" s="27">
-        <v>0.27074999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="F30" s="27">
-        <v>0.10829999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="G30" s="26">
-        <v>7.0489999999999995E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H30" s="26">
-        <v>1.4098E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I30" s="26">
-        <v>8.811E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J30" s="26">
-        <v>1.762E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K30" s="28">
-        <v>1.3555999999999999</v>
-      </c>
-      <c r="L30" s="29">
-        <v>0.27100000000000002</v>
+        <v>0.625</v>
+      </c>
+      <c r="L30" s="28">
+        <v>0.125</v>
       </c>
       <c r="M30" s="28">
-        <v>1.6944999999999999</v>
+        <v>0.78</v>
       </c>
       <c r="N30" s="28">
-        <v>0.33900000000000002</v>
+        <v>0.155</v>
       </c>
       <c r="O30" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2499645339764507</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="P30" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2498226698822528</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="Q30" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.25</v>
+        <v>1.248</v>
       </c>
       <c r="R30" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2509225092250922</v>
+        <v>1.24</v>
       </c>
       <c r="S30" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.39999999999999997</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E31" s="27">
-        <v>0.28499999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="F31" s="27">
-        <v>0.114</v>
+        <v>0.1</v>
       </c>
       <c r="G31" s="26">
-        <v>7.4200000000000004E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H31" s="26">
-        <v>1.484E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I31" s="26">
-        <v>9.2750000000000005E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J31" s="26">
-        <v>1.8550000000000001E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K31" s="28">
-        <v>1.4269000000000001</v>
+        <v>0.625</v>
       </c>
       <c r="L31" s="28">
-        <v>0.28499999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="M31" s="28">
-        <v>1.7836000000000001</v>
+        <v>0.78</v>
       </c>
       <c r="N31" s="28">
-        <v>0.35599999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="O31" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.25</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="P31" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="Q31" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499824795010162</v>
+        <v>1.248</v>
       </c>
       <c r="R31" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.249122807017544</v>
+        <v>1.24</v>
       </c>
       <c r="S31" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
@@ -10098,130 +10049,130 @@
     </row>
     <row r="32" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E32" s="27">
-        <v>0.3135</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F32" s="27">
-        <v>0.12540000000000001</v>
+        <v>0.112</v>
       </c>
       <c r="G32" s="26">
-        <v>8.1400000000000005E-4</v>
+        <v>7.2499999999999995E-4</v>
       </c>
       <c r="H32" s="26">
-        <v>1.628E-4</v>
+        <v>1.45E-4</v>
       </c>
       <c r="I32" s="26">
-        <v>1.018E-3</v>
+        <v>9.0600000000000001E-4</v>
       </c>
       <c r="J32" s="26">
-        <v>2.0350000000000001E-4</v>
+        <v>1.8100000000000001E-4</v>
       </c>
       <c r="K32" s="28">
-        <v>1.57</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="L32" s="28">
-        <v>0.31</v>
+        <v>0.13950000000000001</v>
       </c>
       <c r="M32" s="28">
-        <v>1.96</v>
+        <v>0.87</v>
       </c>
       <c r="N32" s="28">
-        <v>0.39</v>
+        <v>0.17449999999999999</v>
       </c>
       <c r="O32" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.2506142506142506</v>
+        <v>1.2496551724137932</v>
       </c>
       <c r="P32" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.25</v>
+        <v>1.2482758620689656</v>
       </c>
       <c r="Q32" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2484076433121019</v>
+        <v>1.2517985611510791</v>
       </c>
       <c r="R32" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2580645161290323</v>
+        <v>1.25089605734767</v>
       </c>
       <c r="S32" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.4</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E33" s="27">
-        <v>0.33677000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="F33" s="27">
-        <v>0.13471</v>
+        <v>0.1</v>
       </c>
       <c r="G33" s="26">
-        <v>8.7465000000000004E-4</v>
+        <v>6.4999999999999997E-4</v>
       </c>
       <c r="H33" s="26">
-        <v>1.7493000000000001E-4</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="I33" s="26">
-        <v>9.6469999999999998E-4</v>
+        <v>8.0999999999999996E-4</v>
       </c>
       <c r="J33" s="26">
-        <v>2.187E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="K33" s="28">
-        <v>1.6820999999999999</v>
+        <v>0.625</v>
       </c>
       <c r="L33" s="28">
-        <v>0.33639999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="M33" s="28">
-        <v>2.1025999999999998</v>
+        <v>0.78</v>
       </c>
       <c r="N33" s="28">
-        <v>0.42099999999999999</v>
+        <v>0.155</v>
       </c>
       <c r="O33" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- WCU]]/Table4[[#This Row],[Provisioned - WCU]]</f>
-        <v>1.1029554679014462</v>
+        <v>1.2461538461538462</v>
       </c>
       <c r="P33" s="28">
         <f>Table4[[#This Row],[Provisioned_IA- RCU]]/Table4[[#This Row],[Provisioned - RCU]]</f>
-        <v>1.2502143714628708</v>
+        <v>1.2307692307692311</v>
       </c>
       <c r="Q33" s="28">
         <f>Table4[[#This Row],[OD_IA_WRU]]/Table4[[#This Row],[OD_WRU]]</f>
-        <v>1.2499851376255871</v>
+        <v>1.248</v>
       </c>
       <c r="R33" s="28">
         <f>Table4[[#This Row],[OD_IA_RRU]]/Table4[[#This Row],[OD_RRU]]</f>
-        <v>1.2514863258026159</v>
+        <v>1.24</v>
       </c>
       <c r="S33" s="28">
         <f>Table4[[#This Row],[Standard_IA]]/Table4[[#This Row],[Standard]]</f>
-        <v>0.40000593877126822</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="18" x14ac:dyDescent="0.2">

</xml_diff>